<commit_message>
Update to Issue Log
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,8 +11,9 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$57</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$66</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$72</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$57</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$I$66</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="137">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -431,6 +432,39 @@
   </si>
   <si>
     <t xml:space="preserve">EPMD make it reopen in the same state that it closed in </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PixelMap </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">transformGetLineColor uses default divisor of 1000</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">EPMD off on an off pixel caused redraw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since Issue 70 redraw is slower … optimize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This seems to have gone away</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graffiti lines are offset from pixels</t>
   </si>
 </sst>
 </file>
@@ -442,7 +476,7 @@
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY;@"/>
     <numFmt numFmtId="166" formatCode="DD\-MMM"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -472,6 +506,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -652,12 +692,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B72" activeCellId="0" sqref="B72"/>
+      <selection pane="bottomLeft" activeCell="F76" activeCellId="0" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1946,13 +1986,13 @@
         <v>123</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
         <v>68</v>
       </c>
@@ -1994,7 +2034,7 @@
         <v>43657</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2014,7 +2054,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="n">
         <v>72</v>
       </c>
@@ -2028,8 +2068,67 @@
         <v>10</v>
       </c>
     </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E73" s="3" t="n">
+        <v>43657</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E74" s="3" t="n">
+        <v>43657</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E75" s="3" t="n">
+        <v>43657</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E76" s="3" t="n">
+        <v>43657</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I57">
+  <autoFilter ref="A1:I72">
     <filterColumn colId="5">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>

<commit_message>
Issue-86 ControlBase add Typed Listeners, Validators and make adding listeners fluent.
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="158">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -57,43 +57,43 @@
     <t xml:space="preserve">Auto Update Curves</t>
   </si>
   <si>
+    <t xml:space="preserve">CLOSED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you click AUC then the Updated curves button goes away … and the view might be out of date … and you cant refresh it without making a change.  Should track isDirty and do an update if needed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">renemed stuff to Auto </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show graffiti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is an option to show Graftiti … but it only controls the segment grafiti.  Should be able to hide/make transparent the pixels too.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can change the opacity of the grafitti colors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mis matched lines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it would be good to have an option to show where segments are not smoothly matched.  Possibly by coloring the pixel different</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contained project</t>
+  </si>
+  <si>
     <t xml:space="preserve">DONE</t>
   </si>
   <si>
-    <t xml:space="preserve">If you click AUC then the Updated curves button goes away … and the view might be out of date … and you cant refresh it without making a change.  Should track isDirty and do an update if needed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">renemed stuff to Auto </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show graffiti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is an option to show Graftiti … but it only controls the segment grafiti.  Should be able to hide/make transparent the pixels too.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can change the opacity of the grafitti colors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mis matched lines</t>
-  </si>
-  <si>
-    <t xml:space="preserve">it would be good to have an option to show where segments are not smoothly matched.  Possibly by coloring the pixel different</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contained project</t>
-  </si>
-  <si>
     <t xml:space="preserve">Need to have a test image available in the project set so that it can be opened on different platforms</t>
   </si>
   <si>
     <t xml:space="preserve">Proper startup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLOSED</t>
   </si>
   <si>
     <t xml:space="preserve">Need to run this from the javafx application class</t>
@@ -513,6 +513,21 @@
   </si>
   <si>
     <t xml:space="preserve">is there any need for mMouseLastPixelPosition now that graffitiCuror is bing used.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make lines smooth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Join broken lines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change EPMD into state based app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ControlBase </t>
+  </si>
+  <si>
+    <t xml:space="preserve">add Typed Listeners, Validators and make fluent.</t>
   </si>
 </sst>
 </file>
@@ -747,9 +762,9 @@
   <dimension ref="A1:I86"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="bottomLeft" activeCell="H86" activeCellId="0" sqref="H86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -832,13 +847,13 @@
         <v>43658</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -846,7 +861,7 @@
         <v>81</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>0</v>
@@ -855,7 +870,7 @@
         <v>43658</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>18</v>
@@ -875,10 +890,10 @@
         <v>42738</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -886,7 +901,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>1</v>
@@ -895,7 +910,7 @@
         <v>42620</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>23</v>
@@ -916,7 +931,7 @@
         <v>42737</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>25</v>
@@ -939,7 +954,7 @@
         <v>42621</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G8" s="3" t="n">
         <v>42621</v>
@@ -962,7 +977,7 @@
         <v>42736</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>29</v>
@@ -982,7 +997,7 @@
         <v>42605</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G10" s="3" t="n">
         <v>42620</v>
@@ -1011,7 +1026,7 @@
         <v>42624</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G11" s="3" t="n">
         <v>42624</v>
@@ -1034,7 +1049,7 @@
         <v>42624</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G12" s="3" t="n">
         <v>42629</v>
@@ -1057,7 +1072,7 @@
         <v>42624</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G13" s="3" t="n">
         <v>42629</v>
@@ -1080,7 +1095,7 @@
         <v>42629</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G14" s="3" t="n">
         <v>42629</v>
@@ -1100,7 +1115,7 @@
         <v>42736</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1117,7 +1132,7 @@
         <v>42738</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="59.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1137,7 +1152,7 @@
         <v>42620</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>41</v>
@@ -1163,7 +1178,7 @@
         <v>42622</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G18" s="3" t="n">
         <v>42623</v>
@@ -1186,7 +1201,7 @@
         <v>42737</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>46</v>
@@ -1209,7 +1224,7 @@
         <v>42620</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>49</v>
@@ -1232,7 +1247,7 @@
         <v>42738</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1249,7 +1264,7 @@
         <v>42620</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>53</v>
@@ -1272,7 +1287,7 @@
         <v>42620</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>55</v>
@@ -1293,7 +1308,7 @@
         <v>42620</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I24" s="9"/>
     </row>
@@ -1311,7 +1326,7 @@
         <v>42620</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>58</v>
@@ -1331,7 +1346,7 @@
         <v>42620</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>60</v>
@@ -1351,7 +1366,7 @@
         <v>42620</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1368,7 +1383,7 @@
         <v>42620</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1385,7 +1400,7 @@
         <v>42629</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>64</v>
@@ -1405,7 +1420,7 @@
         <v>43657</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>66</v>
@@ -1425,7 +1440,7 @@
         <v>43658</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>68</v>
@@ -1445,7 +1460,7 @@
         <v>43657</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1462,7 +1477,7 @@
         <v>42624</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>71</v>
@@ -1482,7 +1497,7 @@
         <v>42624</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G34" s="3" t="n">
         <v>42624</v>
@@ -1508,7 +1523,7 @@
         <v>42622</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>75</v>
@@ -1528,7 +1543,7 @@
         <v>42622</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>77</v>
@@ -1548,7 +1563,7 @@
         <v>42622</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>79</v>
@@ -1568,7 +1583,7 @@
         <v>42624</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>81</v>
@@ -1588,7 +1603,7 @@
         <v>42622</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>83</v>
@@ -1608,7 +1623,7 @@
         <v>42622</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1625,7 +1640,7 @@
         <v>42658</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>86</v>
@@ -1648,7 +1663,7 @@
         <v>42629</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>87</v>
@@ -1668,7 +1683,7 @@
         <v>42658</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>89</v>
@@ -1685,7 +1700,7 @@
         <v>99</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>91</v>
@@ -1702,7 +1717,7 @@
         <v>99</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>92</v>
@@ -1722,7 +1737,7 @@
         <v>42622</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>94</v>
@@ -1739,7 +1754,7 @@
         <v>99</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G47" s="3" t="n">
         <v>42624</v>
@@ -1765,7 +1780,7 @@
         <v>42622</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="36.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1777,7 +1792,7 @@
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>100</v>
@@ -1793,7 +1808,7 @@
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>102</v>
@@ -1809,7 +1824,7 @@
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>104</v>
@@ -1825,7 +1840,7 @@
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>105</v>
@@ -1841,7 +1856,7 @@
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>106</v>
@@ -1857,7 +1872,7 @@
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>107</v>
@@ -1873,7 +1888,7 @@
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>109</v>
@@ -1889,7 +1904,7 @@
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>111</v>
@@ -1905,7 +1920,7 @@
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>85</v>
@@ -1926,7 +1941,7 @@
         <v>42620</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G58" s="3" t="n">
         <v>42621</v>
@@ -1949,7 +1964,7 @@
         <v>43657</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>115</v>
@@ -1964,7 +1979,7 @@
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>117</v>
@@ -1979,7 +1994,7 @@
         <v>118</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>119</v>
@@ -1994,7 +2009,7 @@
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>121</v>
@@ -2010,7 +2025,7 @@
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>123</v>
@@ -2026,7 +2041,7 @@
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>125</v>
@@ -2042,7 +2057,7 @@
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>127</v>
@@ -2058,7 +2073,7 @@
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>127</v>
@@ -2074,7 +2089,7 @@
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>127</v>
@@ -2090,7 +2105,7 @@
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>131</v>
@@ -2108,7 +2123,7 @@
         <v>43657</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>133</v>
@@ -2125,7 +2140,7 @@
         <v>43657</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>135</v>
@@ -2140,7 +2155,7 @@
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>136</v>
@@ -2160,7 +2175,7 @@
         <v>43657</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>139</v>
@@ -2177,7 +2192,7 @@
         <v>42605</v>
       </c>
       <c r="F73" s="12" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G73" s="3" t="n">
         <v>42605</v>
@@ -2198,7 +2213,7 @@
       </c>
       <c r="D74" s="2"/>
       <c r="F74" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G74" s="3"/>
     </row>
@@ -2211,7 +2226,7 @@
       </c>
       <c r="D75" s="2"/>
       <c r="F75" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G75" s="3"/>
     </row>
@@ -2224,7 +2239,7 @@
       </c>
       <c r="D76" s="2"/>
       <c r="F76" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G76" s="3"/>
     </row>
@@ -2237,7 +2252,7 @@
       </c>
       <c r="D77" s="2"/>
       <c r="F77" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G77" s="3"/>
     </row>
@@ -2252,7 +2267,7 @@
         <v>43657</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2266,7 +2281,7 @@
         <v>43657</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2280,7 +2295,7 @@
         <v>43657</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2294,7 +2309,7 @@
         <v>43658</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2311,13 +2326,80 @@
         <v>43658</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H82" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C83" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E83" s="3" t="n">
+        <v>43658</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C84" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E84" s="3" t="n">
+        <v>43658</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C85" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E85" s="3" t="n">
+        <v>43658</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E86" s="3" t="n">
+        <v>43660</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I81">
     <filterColumn colId="5">

</xml_diff>

<commit_message>
Issue-90 add position to Vertex.  Also added jacoco code coverage and fixed failing tests.
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,10 +11,10 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$90</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$81</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$I$57</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$I$66</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$81</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$90</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$I$57</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$I$66</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="166">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -67,13 +67,16 @@
     <t xml:space="preserve">NONE CODE </t>
   </si>
   <si>
+    <t xml:space="preserve">CLOSED</t>
+  </si>
+  <si>
     <t xml:space="preserve">How to make lines moother … do I need positions in Vertex</t>
   </si>
   <si>
+    <t xml:space="preserve">Ivertex now has an position</t>
+  </si>
+  <si>
     <t xml:space="preserve">Auto Update Curves</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLOSED</t>
   </si>
   <si>
     <t xml:space="preserve">If you click AUC then the Updated curves button goes away … and the view might be out of date … and you cant refresh it without making a change.  Should track isDirty and do an update if needed.</t>
@@ -757,12 +760,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I90"/>
+  <dimension ref="A1:I91"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -842,10 +845,13 @@
         <v>43662</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="48" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -853,7 +859,7 @@
         <v>79</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>0</v>
@@ -862,13 +868,13 @@
         <v>43658</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="36.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -876,7 +882,7 @@
         <v>80</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>0</v>
@@ -885,13 +891,13 @@
         <v>43658</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -899,7 +905,7 @@
         <v>81</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>0</v>
@@ -914,7 +920,7 @@
         <v>10</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -922,7 +928,7 @@
         <v>82</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>0</v>
@@ -934,7 +940,7 @@
         <v>10</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -942,7 +948,7 @@
         <v>83</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0</v>
@@ -962,7 +968,7 @@
         <v>84</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>0</v>
@@ -979,7 +985,7 @@
         <v>85</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>0</v>
@@ -996,7 +1002,7 @@
         <v>86</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>0</v>
@@ -1005,10 +1011,10 @@
         <v>43660</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1016,7 +1022,7 @@
         <v>87</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0</v>
@@ -1033,7 +1039,7 @@
         <v>64</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>1</v>
@@ -1042,10 +1048,10 @@
         <v>42738</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1053,7 +1059,7 @@
         <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>1</v>
@@ -1062,10 +1068,10 @@
         <v>42620</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I14" s="1"/>
     </row>
@@ -1074,7 +1080,7 @@
         <v>63</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>1</v>
@@ -1086,7 +1092,7 @@
         <v>10</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1094,7 +1100,7 @@
         <v>40</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>1</v>
@@ -1106,13 +1112,13 @@
         <v>42621</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G16" s="3" t="n">
         <v>42621</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1120,7 +1126,7 @@
         <v>60</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>1</v>
@@ -1129,10 +1135,10 @@
         <v>42736</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="71" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1140,7 +1146,7 @@
         <v>27</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>1</v>
@@ -1149,16 +1155,16 @@
         <v>42605</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G18" s="3" t="n">
         <v>42620</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1166,7 +1172,7 @@
         <v>52</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>1</v>
@@ -1178,7 +1184,7 @@
         <v>42624</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G19" s="3" t="n">
         <v>42624</v>
@@ -1189,7 +1195,7 @@
         <v>53</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>1</v>
@@ -1201,7 +1207,7 @@
         <v>42624</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G20" s="3" t="n">
         <v>42629</v>
@@ -1212,7 +1218,7 @@
         <v>54</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>1</v>
@@ -1224,7 +1230,7 @@
         <v>42624</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G21" s="3" t="n">
         <v>42629</v>
@@ -1235,7 +1241,7 @@
         <v>55</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>1</v>
@@ -1247,7 +1253,7 @@
         <v>42629</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G22" s="3" t="n">
         <v>42629</v>
@@ -1258,7 +1264,7 @@
         <v>61</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>1</v>
@@ -1275,7 +1281,7 @@
         <v>66</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>1</v>
@@ -1284,7 +1290,7 @@
         <v>42738</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="59.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1292,25 +1298,25 @@
         <v>30</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E25" s="3" t="n">
         <v>42620</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1318,7 +1324,7 @@
         <v>41</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>2</v>
@@ -1330,13 +1336,13 @@
         <v>42622</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G26" s="3" t="n">
         <v>42623</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1344,7 +1350,7 @@
         <v>62</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>2</v>
@@ -1356,7 +1362,7 @@
         <v>10</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1364,13 +1370,13 @@
         <v>31</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>3</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E28" s="3" t="n">
         <v>42620</v>
@@ -1379,10 +1385,10 @@
         <v>10</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1390,7 +1396,7 @@
         <v>65</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>3</v>
@@ -1407,7 +1413,7 @@
         <v>32</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>4</v>
@@ -1419,7 +1425,7 @@
         <v>10</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1427,7 +1433,7 @@
         <v>33</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>5</v>
@@ -1442,7 +1448,7 @@
         <v>10</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I31" s="9"/>
     </row>
@@ -1451,7 +1457,7 @@
         <v>34</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>8</v>
@@ -1469,7 +1475,7 @@
         <v>35</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>9</v>
@@ -1481,7 +1487,7 @@
         <v>10</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1489,7 +1495,7 @@
         <v>38</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>9</v>
@@ -1501,7 +1507,7 @@
         <v>10</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1509,7 +1515,7 @@
         <v>36</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>9</v>
@@ -1526,7 +1532,7 @@
         <v>37</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C36" s="1" t="n">
         <v>9</v>
@@ -1543,7 +1549,7 @@
         <v>57</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C37" s="1" t="n">
         <v>9</v>
@@ -1555,7 +1561,7 @@
         <v>10</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1563,7 +1569,7 @@
         <v>71</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>9</v>
@@ -1575,7 +1581,7 @@
         <v>10</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1583,7 +1589,7 @@
         <v>77</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>9</v>
@@ -1595,7 +1601,7 @@
         <v>10</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1603,7 +1609,7 @@
         <v>73</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>9</v>
@@ -1620,7 +1626,7 @@
         <v>50</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C41" s="1" t="n">
         <v>10</v>
@@ -1632,7 +1638,7 @@
         <v>10</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1640,7 +1646,7 @@
         <v>51</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>10</v>
@@ -1649,13 +1655,13 @@
         <v>42624</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G42" s="3" t="n">
         <v>42624</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1663,7 +1669,7 @@
         <v>46</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>10</v>
@@ -1678,7 +1684,7 @@
         <v>10</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1686,7 +1692,7 @@
         <v>45</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>10</v>
@@ -1698,7 +1704,7 @@
         <v>10</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1706,7 +1712,7 @@
         <v>48</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>10</v>
@@ -1718,7 +1724,7 @@
         <v>10</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1726,7 +1732,7 @@
         <v>49</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>10</v>
@@ -1735,10 +1741,10 @@
         <v>42624</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1746,7 +1752,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>10</v>
@@ -1758,7 +1764,7 @@
         <v>10</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1766,7 +1772,7 @@
         <v>44</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C48" s="1" t="n">
         <v>10</v>
@@ -1783,7 +1789,7 @@
         <v>58</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C49" s="1" t="n">
         <v>99</v>
@@ -1795,7 +1801,7 @@
         <v>10</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1803,7 +1809,7 @@
         <v>56</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C50" s="1" t="n">
         <v>99</v>
@@ -1818,7 +1824,7 @@
         <v>10</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1826,7 +1832,7 @@
         <v>59</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C51" s="1" t="n">
         <v>99</v>
@@ -1838,7 +1844,7 @@
         <v>10</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1846,7 +1852,7 @@
         <v>21</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C52" s="1" t="n">
         <v>99</v>
@@ -1855,7 +1861,7 @@
         <v>10</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1863,7 +1869,7 @@
         <v>20</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C53" s="1" t="n">
         <v>99</v>
@@ -1872,7 +1878,7 @@
         <v>10</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1880,7 +1886,7 @@
         <v>43</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>99</v>
@@ -1892,7 +1898,7 @@
         <v>10</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1900,22 +1906,22 @@
         <v>18</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C55" s="1" t="n">
         <v>99</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G55" s="3" t="n">
         <v>42624</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1923,7 +1929,7 @@
         <v>42</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C56" s="1" t="n">
         <v>99</v>
@@ -1940,7 +1946,7 @@
         <v>88</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>99</v>
@@ -1952,7 +1958,7 @@
         <v>10</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="36.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1960,14 +1966,14 @@
         <v>5</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I58" s="1"/>
     </row>
@@ -1976,14 +1982,14 @@
         <v>26</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I59" s="1"/>
     </row>
@@ -1992,14 +1998,14 @@
         <v>11</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I60" s="1"/>
     </row>
@@ -2008,14 +2014,14 @@
         <v>25</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I61" s="1"/>
     </row>
@@ -2024,14 +2030,14 @@
         <v>24</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I62" s="1"/>
     </row>
@@ -2040,14 +2046,14 @@
         <v>23</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I63" s="1"/>
     </row>
@@ -2056,14 +2062,14 @@
         <v>3</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I64" s="1"/>
     </row>
@@ -2072,14 +2078,14 @@
         <v>7</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I65" s="1"/>
     </row>
@@ -2088,14 +2094,14 @@
         <v>22</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I66" s="1"/>
     </row>
@@ -2104,7 +2110,7 @@
         <v>39</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D67" s="2" t="n">
         <v>27</v>
@@ -2113,16 +2119,16 @@
         <v>42620</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G67" s="3" t="n">
         <v>42621</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2130,16 +2136,16 @@
         <v>74</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E68" s="3" t="n">
         <v>43657</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2147,14 +2153,14 @@
         <v>16</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I69" s="1"/>
     </row>
@@ -2163,13 +2169,13 @@
         <v>67</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2177,14 +2183,14 @@
         <v>4</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I71" s="1"/>
     </row>
@@ -2193,14 +2199,14 @@
         <v>2</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I72" s="1"/>
     </row>
@@ -2209,14 +2215,14 @@
         <v>6</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="I73" s="1"/>
     </row>
@@ -2225,14 +2231,14 @@
         <v>8</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I74" s="1"/>
     </row>
@@ -2241,14 +2247,14 @@
         <v>9</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I75" s="1"/>
     </row>
@@ -2257,14 +2263,14 @@
         <v>10</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I76" s="1"/>
     </row>
@@ -2273,14 +2279,14 @@
         <v>12</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I77" s="1"/>
     </row>
@@ -2289,16 +2295,16 @@
         <v>69</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E78" s="3" t="n">
         <v>43657</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2306,16 +2312,16 @@
         <v>75</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E79" s="3" t="n">
         <v>43657</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2323,17 +2329,17 @@
         <v>19</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2341,16 +2347,16 @@
         <v>68</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E81" s="3" t="n">
         <v>43657</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="48" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2358,22 +2364,22 @@
         <v>28</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E82" s="8" t="n">
         <v>42605</v>
       </c>
       <c r="F82" s="12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G82" s="3" t="n">
         <v>42605</v>
       </c>
       <c r="H82" s="9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I82" s="9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="83" s="1" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2381,11 +2387,11 @@
         <v>13</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D83" s="2"/>
       <c r="F83" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G83" s="3"/>
     </row>
@@ -2394,11 +2400,11 @@
         <v>14</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D84" s="2"/>
       <c r="F84" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G84" s="3"/>
     </row>
@@ -2407,11 +2413,11 @@
         <v>15</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D85" s="2"/>
       <c r="F85" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G85" s="3"/>
     </row>
@@ -2420,11 +2426,11 @@
         <v>17</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D86" s="2"/>
       <c r="F86" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G86" s="3"/>
     </row>
@@ -2433,13 +2439,13 @@
         <v>70</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E87" s="3" t="n">
         <v>43657</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2447,13 +2453,13 @@
         <v>72</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E88" s="3" t="n">
         <v>43657</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2461,13 +2467,13 @@
         <v>76</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E89" s="3" t="n">
         <v>43657</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2475,17 +2481,18 @@
         <v>78</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E90" s="3" t="n">
         <v>43658</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:I90">
+  <autoFilter ref="A1:I81">
     <filterColumn colId="5">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>

<commit_message>
Issue-93 EPMD show graffiti broken
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -12,9 +12,10 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$81</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$90</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$I$57</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$I$66</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$94</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$I$90</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$I$57</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$I$66</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="174">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -58,45 +59,45 @@
     <t xml:space="preserve">IPixelMapTransformSource</t>
   </si>
   <si>
+    <t xml:space="preserve">CLOSED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remove PixelChain dependency on IpixelMapTransformSource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Too hard as this is in Segment too and it makes the parameter lists too long.  Did do code coverage and some tidy ups whilst looking at code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NONE CODE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How to make lines moother … do I need positions in Vertex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto Update Curves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you click AUC then the Updated curves button goes away … and the view might be out of date … and you cant refresh it without making a change.  Should track isDirty and do an update if needed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">renemed stuff to Auto </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show graffiti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is an option to show Graftiti … but it only controls the segment grafiti.  Should be able to hide/make transparent the pixels too.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can change the opacity of the grafitti colors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mis matched lines</t>
+  </si>
+  <si>
     <t xml:space="preserve">OPEN</t>
   </si>
   <si>
-    <t xml:space="preserve">remove PixelChain dependency on IpixelMapTransformSource</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NONE CODE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLOSED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How to make lines moother … do I need positions in Vertex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ivertex now has an position</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auto Update Curves</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If you click AUC then the Updated curves button goes away … and the view might be out of date … and you cant refresh it without making a change.  Should track isDirty and do an update if needed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">renemed stuff to Auto </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show graffiti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There is an option to show Graftiti … but it only controls the segment grafiti.  Should be able to hide/make transparent the pixels too.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can change the opacity of the grafitti colors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mis matched lines</t>
-  </si>
-  <si>
     <t xml:space="preserve">it would be good to have an option to show where segments are not smoothly matched.  Possibly by coloring the pixel different</t>
   </si>
   <si>
@@ -122,6 +123,30 @@
   </si>
   <si>
     <t xml:space="preserve">Fix errors that prevent mvn clean build</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counter failure if max not set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should have two interfaces … Icounter, ImaxCounter … return ImaxCounter when .withMax() called </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CET Update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When performing a LineTolerance change in CET whilst it is still calculating it is possible to open the EditPixelMap dialog … needs to have progress and disable button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPMD show graffiti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does not work immediately … only on next redraw …. needs to trigger redraw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CET curve preference per thickness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Think about if this is a good idea</t>
   </si>
   <si>
     <t xml:space="preserve">Contained project</t>
@@ -760,12 +785,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I91"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -811,7 +836,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="48" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>89</v>
       </c>
@@ -830,13 +855,16 @@
       <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>90</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>-1</v>
@@ -845,13 +873,10 @@
         <v>43662</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="48" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -859,7 +884,7 @@
         <v>79</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>0</v>
@@ -868,13 +893,13 @@
         <v>43658</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="36.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -882,7 +907,7 @@
         <v>80</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>0</v>
@@ -891,13 +916,13 @@
         <v>43658</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -905,7 +930,7 @@
         <v>81</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>0</v>
@@ -917,7 +942,7 @@
         <v>43658</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>23</v>
@@ -937,7 +962,7 @@
         <v>43658</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>25</v>
@@ -960,7 +985,7 @@
         <v>43658</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -977,7 +1002,7 @@
         <v>43658</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -994,7 +1019,7 @@
         <v>43658</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1011,7 +1036,7 @@
         <v>43660</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>30</v>
@@ -1031,119 +1056,112 @@
         <v>43662</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>42738</v>
+        <v>43664</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="2" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3" t="n">
+        <v>43664</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E14" s="7" t="n">
-        <v>42620</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="2" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
-        <v>63</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3" t="n">
+        <v>43664</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" s="3" t="n">
-        <v>42737</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="2" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3" t="n">
+        <v>43664</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C16" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D16" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="E16" s="3" t="n">
-        <v>42621</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="3" t="n">
-        <v>42621</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>42736</v>
+        <v>42738</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="71" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>43</v>
@@ -1151,48 +1169,40 @@
       <c r="C18" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E18" s="3" t="n">
-        <v>42605</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="3" t="n">
+      <c r="E18" s="7" t="n">
         <v>42620</v>
       </c>
-      <c r="H18" s="9" t="s">
+      <c r="F18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
-        <v>52</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D19" s="2" t="n">
-        <v>30</v>
-      </c>
       <c r="E19" s="3" t="n">
-        <v>42624</v>
+        <v>42737</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="3" t="n">
-        <v>42624</v>
+        <v>22</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>47</v>
@@ -1204,512 +1214,521 @@
         <v>30</v>
       </c>
       <c r="E20" s="3" t="n">
-        <v>42624</v>
+        <v>42621</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G20" s="3" t="n">
-        <v>42629</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>42621</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D21" s="2" t="n">
-        <v>30</v>
-      </c>
       <c r="E21" s="3" t="n">
-        <v>42624</v>
+        <v>42736</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="3" t="n">
-        <v>42629</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="71" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="2" t="n">
+      <c r="E22" s="3" t="n">
+        <v>42605</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="3" t="n">
+        <v>42620</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="E22" s="3" t="n">
-        <v>42629</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="3" t="n">
-        <v>42629</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
-        <v>61</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="D23" s="2" t="n">
+        <v>30</v>
+      </c>
       <c r="E23" s="3" t="n">
-        <v>42736</v>
+        <v>42624</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="G23" s="3" t="n">
+        <v>42624</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="D24" s="2" t="n">
+        <v>30</v>
+      </c>
       <c r="E24" s="3" t="n">
-        <v>42738</v>
+        <v>42624</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="59.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="G24" s="3" t="n">
+        <v>42629</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="E25" s="3" t="n">
-        <v>42620</v>
+        <v>42624</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I25" s="10" t="s">
-        <v>55</v>
+        <v>10</v>
+      </c>
+      <c r="G25" s="3" t="n">
+        <v>42629</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="E26" s="3" t="n">
-        <v>42622</v>
+        <v>42629</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G26" s="3" t="n">
-        <v>42623</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>42629</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3" t="n">
+        <v>42736</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" s="3" t="n">
+        <v>42738</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="59.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E27" s="3" t="n">
+      <c r="D29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="3" t="n">
+        <v>42620</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="E30" s="3" t="n">
+        <v>42622</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="3" t="n">
+        <v>42623</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E31" s="3" t="n">
         <v>42737</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
+      <c r="F31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="1" t="n">
+      <c r="B32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E28" s="3" t="n">
-        <v>42620</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="I28" s="10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C29" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E29" s="3" t="n">
-        <v>42738</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E30" s="3" t="n">
-        <v>42620</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D31" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="E31" s="3" t="n">
-        <v>42620</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I31" s="9"/>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B32" s="1" t="s">
+      <c r="D32" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="C32" s="1" t="n">
-        <v>8</v>
       </c>
       <c r="E32" s="3" t="n">
         <v>42620</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I32" s="9"/>
-    </row>
-    <row r="33" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>22</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E33" s="3" t="n">
-        <v>42620</v>
+        <v>42738</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E34" s="3" t="n">
         <v>42620</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="D35" s="2" t="n">
+        <v>30</v>
       </c>
       <c r="E35" s="3" t="n">
         <v>42620</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I35" s="9"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E36" s="3" t="n">
         <v>42620</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="I36" s="9"/>
     </row>
     <row r="37" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C37" s="1" t="n">
         <v>9</v>
       </c>
       <c r="E37" s="3" t="n">
-        <v>42629</v>
+        <v>42620</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>9</v>
       </c>
       <c r="E38" s="3" t="n">
-        <v>43657</v>
+        <v>42620</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
-        <v>77</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>80</v>
+        <v>36</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>9</v>
       </c>
       <c r="E39" s="3" t="n">
-        <v>43658</v>
+        <v>42620</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>9</v>
       </c>
       <c r="E40" s="3" t="n">
+        <v>42620</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E41" s="3" t="n">
+        <v>42629</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E42" s="3" t="n">
         <v>43657</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="E41" s="3" t="n">
-        <v>42624</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
-        <v>51</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C42" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="E42" s="3" t="n">
-        <v>42624</v>
-      </c>
       <c r="F42" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G42" s="3" t="n">
-        <v>42624</v>
+        <v>22</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>88</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="D43" s="2" t="n">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="E43" s="3" t="n">
-        <v>42622</v>
+        <v>43658</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E44" s="3" t="n">
-        <v>42622</v>
+        <v>43657</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>91</v>
@@ -1718,10 +1737,10 @@
         <v>10</v>
       </c>
       <c r="E45" s="3" t="n">
-        <v>42622</v>
+        <v>42624</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>92</v>
@@ -1729,7 +1748,7 @@
     </row>
     <row r="46" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>93</v>
@@ -1741,7 +1760,10 @@
         <v>42624</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>33</v>
+        <v>10</v>
+      </c>
+      <c r="G46" s="3" t="n">
+        <v>42624</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>94</v>
@@ -1749,7 +1771,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>95</v>
@@ -1757,19 +1779,22 @@
       <c r="C47" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="D47" s="2" t="n">
+        <v>31</v>
+      </c>
       <c r="E47" s="3" t="n">
         <v>42622</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>97</v>
@@ -1781,152 +1806,155 @@
         <v>42622</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="E49" s="3" t="n">
-        <v>42658</v>
+        <v>42622</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>99</v>
-      </c>
-      <c r="D50" s="2" t="n">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E50" s="3" t="n">
-        <v>42629</v>
+        <v>42624</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>41</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="E51" s="3" t="n">
-        <v>42658</v>
+        <v>42622</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>99</v>
+        <v>10</v>
+      </c>
+      <c r="E52" s="3" t="n">
+        <v>42622</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C53" s="1" t="n">
         <v>99</v>
       </c>
+      <c r="E53" s="3" t="n">
+        <v>42658</v>
+      </c>
       <c r="F53" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>99</v>
       </c>
+      <c r="D54" s="2" t="n">
+        <v>55</v>
+      </c>
       <c r="E54" s="3" t="n">
-        <v>42622</v>
+        <v>42629</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>22</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C55" s="1" t="n">
         <v>99</v>
       </c>
+      <c r="E55" s="3" t="n">
+        <v>42658</v>
+      </c>
       <c r="F55" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G55" s="3" t="n">
-        <v>42624</v>
+        <v>22</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="I55" s="2" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>111</v>
@@ -1934,292 +1962,307 @@
       <c r="C56" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="E56" s="3" t="n">
-        <v>42622</v>
-      </c>
       <c r="F56" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
-        <v>88</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>112</v>
+        <v>20</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="E57" s="3" t="n">
-        <v>43662</v>
-      </c>
       <c r="F57" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H57" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="36.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E58" s="1"/>
+      <c r="C58" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="E58" s="3" t="n">
+        <v>42622</v>
+      </c>
       <c r="F58" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I58" s="1"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E59" s="1"/>
+      <c r="C59" s="1" t="n">
+        <v>99</v>
+      </c>
       <c r="F59" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H59" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G59" s="3" t="n">
+        <v>42624</v>
+      </c>
+      <c r="H59" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="I59" s="1"/>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I59" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E60" s="1"/>
+        <v>119</v>
+      </c>
+      <c r="C60" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="E60" s="3" t="n">
+        <v>42622</v>
+      </c>
       <c r="F60" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="I60" s="1"/>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E61" s="1"/>
+        <v>88</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C61" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="E61" s="3" t="n">
+        <v>43662</v>
+      </c>
       <c r="F61" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="I61" s="1"/>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="36.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>121</v>
+        <v>10</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="I62" s="1"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="I63" s="1"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="I64" s="1"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I65" s="1"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>98</v>
+        <v>129</v>
       </c>
       <c r="I66" s="1"/>
     </row>
-    <row r="67" customFormat="false" ht="36.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="n">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D67" s="2" t="n">
-        <v>27</v>
-      </c>
-      <c r="E67" s="3" t="n">
-        <v>42620</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="E67" s="1"/>
       <c r="F67" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G67" s="3" t="n">
-        <v>42621</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="I67" s="2" t="s">
-        <v>128</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I67" s="1"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
-        <v>74</v>
+        <v>3</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E68" s="3" t="n">
-        <v>43657</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="E68" s="1"/>
       <c r="F68" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>130</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I68" s="1"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="n">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="I69" s="1"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="n">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>133</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="E70" s="1"/>
       <c r="F70" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H70" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I70" s="1"/>
+    </row>
+    <row r="71" customFormat="false" ht="36.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="n">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D71" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="E71" s="3" t="n">
+        <v>42620</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G71" s="3" t="n">
+        <v>42621</v>
+      </c>
+      <c r="H71" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H71" s="1" t="s">
+      <c r="I71" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="I71" s="1"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="n">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E72" s="1"/>
+      <c r="E72" s="3" t="n">
+        <v>43657</v>
+      </c>
       <c r="F72" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H72" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H72" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="I72" s="1"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>140</v>
@@ -2228,269 +2271,330 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="n">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E74" s="1"/>
       <c r="F74" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H74" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H74" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="I74" s="1"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>143</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="I75" s="1"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="I76" s="1"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I77" s="1"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="n">
-        <v>69</v>
+        <v>8</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E78" s="3" t="n">
-        <v>43657</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="E78" s="1"/>
       <c r="F78" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H78" s="2" t="s">
-        <v>148</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="I78" s="1"/>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="n">
-        <v>75</v>
+        <v>9</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E79" s="3" t="n">
-        <v>43657</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="E79" s="1"/>
       <c r="F79" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H79" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H79" s="1" t="s">
         <v>150</v>
       </c>
+      <c r="I79" s="1"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>103</v>
+        <v>152</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="I80" s="1" t="s">
-        <v>152</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="I80" s="1"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="n">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E81" s="3" t="n">
-        <v>43657</v>
-      </c>
+      <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="82" customFormat="false" ht="48" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I81" s="1"/>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="n">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E82" s="8" t="n">
+      <c r="E82" s="3" t="n">
+        <v>43657</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E83" s="3" t="n">
+        <v>43657</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E85" s="3" t="n">
+        <v>43657</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="48" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E86" s="8" t="n">
         <v>42605</v>
       </c>
-      <c r="F82" s="12" t="s">
+      <c r="F86" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G86" s="3" t="n">
+        <v>42605</v>
+      </c>
+      <c r="H86" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="I86" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="87" s="1" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="G82" s="3" t="n">
-        <v>42605</v>
-      </c>
-      <c r="H82" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="I82" s="9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="83" s="1" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D83" s="2"/>
-      <c r="F83" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G83" s="3"/>
-    </row>
-    <row r="84" s="1" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="n">
+      <c r="B87" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D87" s="2"/>
+      <c r="F87" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G87" s="3"/>
+    </row>
+    <row r="88" s="1" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B84" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D84" s="2"/>
-      <c r="F84" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G84" s="3"/>
-    </row>
-    <row r="85" s="1" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1" t="n">
+      <c r="B88" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D88" s="2"/>
+      <c r="F88" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G88" s="3"/>
+    </row>
+    <row r="89" s="1" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B85" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D85" s="2"/>
-      <c r="F85" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G85" s="3"/>
-    </row>
-    <row r="86" s="1" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="n">
+      <c r="B89" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D89" s="2"/>
+      <c r="F89" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G89" s="3"/>
+    </row>
+    <row r="90" s="1" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B86" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D86" s="2"/>
-      <c r="F86" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G86" s="3"/>
-    </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="n">
+      <c r="B90" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D90" s="2"/>
+      <c r="F90" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G90" s="3"/>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E87" s="3" t="n">
+      <c r="B91" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E91" s="3" t="n">
         <v>43657</v>
       </c>
-      <c r="F87" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="n">
+      <c r="F91" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="n">
         <v>72</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E88" s="3" t="n">
+      <c r="B92" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E92" s="3" t="n">
         <v>43657</v>
       </c>
-      <c r="F88" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="n">
+      <c r="F92" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E89" s="3" t="n">
+      <c r="B93" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E93" s="3" t="n">
         <v>43657</v>
       </c>
-      <c r="F89" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="n">
+      <c r="F93" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="n">
         <v>78</v>
       </c>
-      <c r="B90" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E90" s="3" t="n">
+      <c r="B94" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E94" s="3" t="n">
         <v>43658</v>
       </c>
-      <c r="F90" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="F94" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I81">
     <filterColumn colId="5">

</xml_diff>

<commit_message>
Issue-91 Counter failure if max not set
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -790,7 +790,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1073,7 +1073,7 @@
         <v>43664</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Issue-96 Fix typo grafitti -> graffiti
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,11 +11,12 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$81</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$94</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$I$90</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$I$57</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$I$66</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$94</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$95</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$I$81</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$I$90</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$I$57</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$I$66</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="177">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -56,6 +57,15 @@
     <t xml:space="preserve">Response / Test</t>
   </si>
   <si>
+    <t xml:space="preserve">CET Update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When performing a LineTolerance change in CET whilst it is still calculating it is possible to open the EditPixelMap dialog … needs to have progress and disable button</t>
+  </si>
+  <si>
     <t xml:space="preserve">IPixelMapTransformSource</t>
   </si>
   <si>
@@ -74,6 +84,9 @@
     <t xml:space="preserve">How to make lines moother … do I need positions in Vertex</t>
   </si>
   <si>
+    <t xml:space="preserve">Different Curve tolerances</t>
+  </si>
+  <si>
     <t xml:space="preserve">Auto Update Curves</t>
   </si>
   <si>
@@ -95,9 +108,6 @@
     <t xml:space="preserve">Mis matched lines</t>
   </si>
   <si>
-    <t xml:space="preserve">OPEN</t>
-  </si>
-  <si>
     <t xml:space="preserve">it would be good to have an option to show where segments are not smoothly matched.  Possibly by coloring the pixel different</t>
   </si>
   <si>
@@ -113,9 +123,6 @@
     <t xml:space="preserve">Join broken lines</t>
   </si>
   <si>
-    <t xml:space="preserve">Change EPMD into state based app</t>
-  </si>
-  <si>
     <t xml:space="preserve">ControlBase </t>
   </si>
   <si>
@@ -129,12 +136,6 @@
   </si>
   <si>
     <t xml:space="preserve">Should have two interfaces … Icounter, ImaxCounter … return ImaxCounter when .withMax() called </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CET Update</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When performing a LineTolerance change in CET whilst it is still calculating it is possible to open the EditPixelMap dialog … needs to have progress and disable button</t>
   </si>
   <si>
     <t xml:space="preserve">EPMD show graffiti</t>
@@ -357,6 +358,12 @@
     <t xml:space="preserve">Platform Runlater</t>
   </si>
   <si>
+    <t xml:space="preserve">Change EPMD into state based app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not important at the moment</t>
+  </si>
+  <si>
     <t xml:space="preserve">NamedTabs</t>
   </si>
   <si>
@@ -560,6 +567,9 @@
   </si>
   <si>
     <t xml:space="preserve">CannyTransform generate egdes needs to disable EditPixels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fix typo grafitti → graffiti</t>
   </si>
 </sst>
 </file>
@@ -785,12 +795,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I94"/>
+  <dimension ref="A1:I96"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="G96" activeCellId="0" sqref="G96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -836,18 +846,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="48" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>43662</v>
+        <v>43664</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
@@ -855,16 +865,13 @@
       <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="48" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>90</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>-1</v>
@@ -873,87 +880,81 @@
         <v>43662</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="48" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>43658</v>
+        <v>43662</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="36.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>43658</v>
+        <v>43664</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="2" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="48" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>81</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D6" s="2" t="n">
-        <v>90</v>
-      </c>
       <c r="E6" s="3" t="n">
         <v>43658</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="36.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>82</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>0</v>
@@ -962,35 +963,41 @@
         <v>43658</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>83</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E8" s="3" t="n">
         <v>43658</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>27</v>
@@ -1002,15 +1009,18 @@
         <v>43658</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>0</v>
@@ -1019,32 +1029,29 @@
         <v>43658</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>0</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>43660</v>
+        <v>43658</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>31</v>
@@ -1053,35 +1060,35 @@
         <v>0</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>43662</v>
+        <v>43660</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>43664</v>
+        <v>43662</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>34</v>
@@ -1093,13 +1100,13 @@
         <v>43664</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>93</v>
       </c>
@@ -1113,7 +1120,7 @@
         <v>43664</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>37</v>
@@ -1133,7 +1140,7 @@
         <v>43664</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>39</v>
@@ -1173,7 +1180,7 @@
         <v>42620</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>44</v>
@@ -1194,7 +1201,7 @@
         <v>42737</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>46</v>
@@ -1217,7 +1224,7 @@
         <v>42621</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G20" s="3" t="n">
         <v>42621</v>
@@ -1240,7 +1247,7 @@
         <v>42736</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>50</v>
@@ -1260,7 +1267,7 @@
         <v>42605</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G22" s="3" t="n">
         <v>42620</v>
@@ -1289,7 +1296,7 @@
         <v>42624</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G23" s="3" t="n">
         <v>42624</v>
@@ -1312,7 +1319,7 @@
         <v>42624</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G24" s="3" t="n">
         <v>42629</v>
@@ -1335,7 +1342,7 @@
         <v>42624</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G25" s="3" t="n">
         <v>42629</v>
@@ -1358,7 +1365,7 @@
         <v>42629</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G26" s="3" t="n">
         <v>42629</v>
@@ -1378,7 +1385,7 @@
         <v>42736</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1415,7 +1422,7 @@
         <v>42620</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>62</v>
@@ -1441,7 +1448,7 @@
         <v>42622</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G30" s="3" t="n">
         <v>42623</v>
@@ -1464,7 +1471,7 @@
         <v>42737</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>67</v>
@@ -1487,7 +1494,7 @@
         <v>42620</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>70</v>
@@ -1510,7 +1517,7 @@
         <v>42738</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1527,7 +1534,7 @@
         <v>42620</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>74</v>
@@ -1550,7 +1557,7 @@
         <v>42620</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>76</v>
@@ -1571,7 +1578,7 @@
         <v>42620</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I36" s="9"/>
     </row>
@@ -1589,7 +1596,7 @@
         <v>42620</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>79</v>
@@ -1609,7 +1616,7 @@
         <v>42620</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>81</v>
@@ -1629,7 +1636,7 @@
         <v>42620</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1646,7 +1653,7 @@
         <v>42620</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1663,7 +1670,7 @@
         <v>42629</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>85</v>
@@ -1683,7 +1690,7 @@
         <v>43657</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>87</v>
@@ -1703,7 +1710,7 @@
         <v>43658</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>89</v>
@@ -1723,7 +1730,7 @@
         <v>43657</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1740,7 +1747,7 @@
         <v>42624</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>92</v>
@@ -1760,7 +1767,7 @@
         <v>42624</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G46" s="3" t="n">
         <v>42624</v>
@@ -1786,7 +1793,7 @@
         <v>42622</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>96</v>
@@ -1806,7 +1813,7 @@
         <v>42622</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>98</v>
@@ -1826,7 +1833,7 @@
         <v>42622</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>100</v>
@@ -1866,7 +1873,7 @@
         <v>42622</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>104</v>
@@ -1886,12 +1893,12 @@
         <v>42622</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>106</v>
@@ -1900,61 +1907,61 @@
         <v>99</v>
       </c>
       <c r="E53" s="3" t="n">
-        <v>42658</v>
+        <v>43658</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H53" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="D54" s="2" t="n">
-        <v>55</v>
-      </c>
       <c r="E54" s="3" t="n">
-        <v>42629</v>
+        <v>42658</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="C55" s="1" t="n">
         <v>99</v>
       </c>
+      <c r="D55" s="2" t="n">
+        <v>55</v>
+      </c>
       <c r="E55" s="3" t="n">
-        <v>42658</v>
+        <v>42629</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H55" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H55" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>111</v>
@@ -1962,8 +1969,11 @@
       <c r="C56" s="1" t="n">
         <v>99</v>
       </c>
+      <c r="E56" s="3" t="n">
+        <v>42658</v>
+      </c>
       <c r="F56" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H56" s="2" t="s">
         <v>112</v>
@@ -1971,44 +1981,41 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>99</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C58" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="E58" s="3" t="n">
-        <v>42622</v>
-      </c>
       <c r="F58" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>116</v>
@@ -2016,98 +2023,102 @@
       <c r="C59" s="1" t="n">
         <v>99</v>
       </c>
+      <c r="E59" s="3" t="n">
+        <v>42622</v>
+      </c>
       <c r="F59" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="G59" s="3" t="n">
-        <v>42624</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="I59" s="2" t="s">
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="C60" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="E60" s="3" t="n">
-        <v>42622</v>
-      </c>
       <c r="F60" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
+      </c>
+      <c r="G60" s="3" t="n">
+        <v>42624</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
-        <v>88</v>
-      </c>
-      <c r="B61" s="11" t="s">
-        <v>120</v>
+        <v>42</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="C61" s="1" t="n">
         <v>99</v>
       </c>
       <c r="E61" s="3" t="n">
+        <v>42622</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C62" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="E62" s="3" t="n">
         <v>43662</v>
       </c>
-      <c r="F61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="36.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="n">
+      <c r="F62" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="36.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="n">
         <v>5</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="I62" s="1"/>
-    </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="n">
-        <v>26</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>124</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H63" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H63" s="2" t="s">
         <v>125</v>
       </c>
       <c r="I63" s="1"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>126</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>127</v>
@@ -2116,62 +2127,62 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I65" s="1"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I66" s="1"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I67" s="1"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>132</v>
@@ -2180,14 +2191,14 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>133</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>134</v>
@@ -2196,119 +2207,119 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>111</v>
+        <v>135</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>106</v>
+        <v>136</v>
       </c>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" customFormat="false" ht="36.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I71" s="1"/>
+    </row>
+    <row r="72" customFormat="false" ht="36.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D71" s="2" t="n">
+      <c r="D72" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="E71" s="3" t="n">
+      <c r="E72" s="3" t="n">
         <v>42620</v>
       </c>
-      <c r="F71" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G71" s="3" t="n">
+      <c r="F72" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G72" s="3" t="n">
         <v>42621</v>
       </c>
-      <c r="H71" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="I71" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="n">
-        <v>74</v>
-      </c>
-      <c r="B72" s="1" t="s">
+      <c r="H72" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="E72" s="3" t="n">
-        <v>43657</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H72" s="2" t="s">
+      <c r="I72" s="2" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="n">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E73" s="1"/>
+      <c r="E73" s="3" t="n">
+        <v>43657</v>
+      </c>
       <c r="F73" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H73" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H73" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="I73" s="1"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="n">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>141</v>
       </c>
+      <c r="E74" s="1"/>
       <c r="F74" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H74" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H74" s="1" t="s">
         <v>142</v>
       </c>
+      <c r="I74" s="1"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="n">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E75" s="1"/>
       <c r="F75" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H75" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H75" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="I75" s="1"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>146</v>
@@ -2317,14 +2328,14 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>147</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>148</v>
@@ -2333,14 +2344,14 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>149</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>150</v>
@@ -2349,72 +2360,71 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>151</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="I79" s="1"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="I80" s="1"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I81" s="1"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="n">
-        <v>69</v>
+        <v>12</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E82" s="3" t="n">
-        <v>43657</v>
-      </c>
+      <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H82" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H82" s="1" t="s">
         <v>156</v>
       </c>
+      <c r="I82" s="1"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="n">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>157</v>
@@ -2423,7 +2433,7 @@
         <v>43657</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H83" s="2" t="s">
         <v>158</v>
@@ -2431,172 +2441,206 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="n">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E84" s="1"/>
+        <v>159</v>
+      </c>
+      <c r="E84" s="3" t="n">
+        <v>43657</v>
+      </c>
       <c r="F84" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H84" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I84" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H84" s="2" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="n">
         <v>68</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E85" s="3" t="n">
-        <v>43657</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H85" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="48" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="n">
-        <v>28</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E86" s="8" t="n">
+      <c r="E86" s="3" t="n">
+        <v>43657</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="48" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E87" s="8" t="n">
         <v>42605</v>
       </c>
-      <c r="F86" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G86" s="3" t="n">
+      <c r="F87" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G87" s="3" t="n">
         <v>42605</v>
       </c>
-      <c r="H86" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="I86" s="9" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="87" s="1" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B87" s="1" t="s">
+      <c r="H87" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="D87" s="2"/>
-      <c r="F87" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G87" s="3"/>
+      <c r="I87" s="9" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="88" s="1" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D88" s="2"/>
       <c r="F88" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G88" s="3"/>
     </row>
     <row r="89" s="1" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D89" s="2"/>
       <c r="F89" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G89" s="3"/>
     </row>
     <row r="90" s="1" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D90" s="2"/>
       <c r="F90" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G90" s="3"/>
     </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" s="1" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="n">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="E91" s="3" t="n">
-        <v>43657</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="D91" s="2"/>
       <c r="F91" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="G91" s="3"/>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="n">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E92" s="3" t="n">
         <v>43657</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="n">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E93" s="3" t="n">
         <v>43657</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E94" s="3" t="n">
+        <v>43657</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="n">
         <v>78</v>
       </c>
-      <c r="B94" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E94" s="3" t="n">
+      <c r="B95" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E95" s="3" t="n">
         <v>43658</v>
       </c>
-      <c r="F94" s="1" t="s">
-        <v>10</v>
+      <c r="F95" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C96" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="E96" s="3" t="n">
+        <v>43665</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I81">
+  <autoFilter ref="A1:I94">
     <filterColumn colId="5">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>

<commit_message>
BREAKING CHANGES DO NOT MERGE
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="178">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -569,7 +569,10 @@
     <t xml:space="preserve">CannyTransform generate egdes needs to disable EditPixels</t>
   </si>
   <si>
-    <t xml:space="preserve">Fix typo grafitti → graffiti</t>
+    <t xml:space="preserve">fix typo grafitti → grafitti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fix .gitignore</t>
   </si>
 </sst>
 </file>
@@ -795,12 +798,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I96"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G96" activeCellId="0" sqref="G96"/>
+      <selection pane="bottomLeft" activeCell="F97" activeCellId="0" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2622,7 +2625,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="n">
         <v>96</v>
       </c>
@@ -2630,13 +2633,30 @@
         <v>176</v>
       </c>
       <c r="C96" s="1" t="n">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="E96" s="3" t="n">
         <v>43665</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E97" s="3" t="n">
+        <v>43665</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue-83 added mid section refinement
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,8 +11,9 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$94</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$95</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$98</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$94</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$I$95</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$I$81</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$I$90</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$I$57</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="179">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -57,12 +58,21 @@
     <t xml:space="preserve">Response / Test</t>
   </si>
   <si>
+    <t xml:space="preserve">Make lines smooth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make PixelChain truly immutbale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create ImmutableVector</t>
+  </si>
+  <si>
     <t xml:space="preserve">CET Update</t>
   </si>
   <si>
-    <t xml:space="preserve">OPEN</t>
-  </si>
-  <si>
     <t xml:space="preserve">When performing a LineTolerance change in CET whilst it is still calculating it is possible to open the EditPixelMap dialog … needs to have progress and disable button</t>
   </si>
   <si>
@@ -115,9 +125,6 @@
   </si>
   <si>
     <t xml:space="preserve">is there any need for mMouseLastPixelPosition now that graffitiCuror is bing used.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Make lines smooth</t>
   </si>
   <si>
     <t xml:space="preserve">Join broken lines</t>
@@ -412,6 +419,9 @@
     <t xml:space="preserve">@NotNull different code is generated in IntelliJ to Maven hence leads to different test results</t>
   </si>
   <si>
+    <t xml:space="preserve">Fix typo grafitti → graffiti</t>
+  </si>
+  <si>
     <t xml:space="preserve">addView</t>
   </si>
   <si>
@@ -567,9 +577,6 @@
   </si>
   <si>
     <t xml:space="preserve">CannyTransform generate egdes needs to disable EditPixels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fix typo grafitti → graffiti</t>
   </si>
 </sst>
 </file>
@@ -795,12 +802,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I96"/>
+  <dimension ref="A1:I98"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G96" activeCellId="0" sqref="G96"/>
+      <selection pane="bottomLeft" activeCell="E98" activeCellId="0" sqref="E98:F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -846,78 +853,69 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="1" t="n">
+        <v>-10</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>43658</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>-9</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>98</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>43668</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>-9</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>43668</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="n">
         <v>-2</v>
-      </c>
-      <c r="E2" s="3" t="n">
-        <v>43664</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="48" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>89</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E3" s="3" t="n">
-        <v>43662</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>90</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E4" s="3" t="n">
-        <v>43662</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>95</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>-1</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>43664</v>
@@ -925,82 +923,76 @@
       <c r="F5" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="H5" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="48" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>43662</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>43662</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>43664</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="48" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
         <v>79</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3" t="n">
-        <v>43658</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="36.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>80</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3" t="n">
-        <v>43658</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>81</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>90</v>
-      </c>
-      <c r="E8" s="3" t="n">
-        <v>43658</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
-        <v>82</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>0</v>
@@ -1009,18 +1001,21 @@
         <v>43658</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="36.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>0</v>
@@ -1029,109 +1024,118 @@
         <v>43658</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="D11" s="2" t="n">
+        <v>90</v>
+      </c>
       <c r="E11" s="3" t="n">
         <v>43658</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H11" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>43660</v>
+        <v>43658</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H12" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
-        <v>87</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>43662</v>
+        <v>43658</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>0</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>43664</v>
+        <v>43660</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H14" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
-        <v>93</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>0</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>43664</v>
+        <v>43662</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0</v>
@@ -1140,194 +1144,188 @@
         <v>43664</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3" t="n">
+        <v>43664</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3" t="n">
+        <v>43664</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E17" s="3" t="n">
-        <v>42738</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H17" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E18" s="7" t="n">
-        <v>42620</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
-        <v>63</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>42737</v>
+        <v>42738</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="E20" s="3" t="n">
-        <v>42621</v>
+      <c r="E20" s="7" t="n">
+        <v>42620</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="3" t="n">
-        <v>42621</v>
+        <v>16</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>46</v>
+      </c>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>42736</v>
+        <v>42737</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="71" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="D22" s="2" t="n">
+        <v>30</v>
+      </c>
       <c r="E22" s="3" t="n">
-        <v>42605</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>13</v>
+        <v>42621</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="G22" s="3" t="n">
-        <v>42620</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>42621</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D23" s="2" t="n">
-        <v>30</v>
-      </c>
       <c r="E23" s="3" t="n">
-        <v>42624</v>
+        <v>42736</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="3" t="n">
-        <v>42624</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="71" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D24" s="2" t="n">
-        <v>30</v>
-      </c>
       <c r="E24" s="3" t="n">
-        <v>42624</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>13</v>
+        <v>42605</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="G24" s="3" t="n">
-        <v>42629</v>
+        <v>42620</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>56</v>
@@ -1342,15 +1340,15 @@
         <v>42624</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G25" s="3" t="n">
-        <v>42629</v>
+        <v>42624</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>57</v>
@@ -1359,21 +1357,21 @@
         <v>1</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="E26" s="3" t="n">
-        <v>42629</v>
+        <v>42624</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G26" s="3" t="n">
         <v>42629</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>58</v>
@@ -1381,16 +1379,22 @@
       <c r="C27" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="D27" s="2" t="n">
+        <v>30</v>
+      </c>
       <c r="E27" s="3" t="n">
-        <v>42736</v>
+        <v>42624</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="G27" s="3" t="n">
+        <v>42629</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>59</v>
@@ -1398,137 +1402,137 @@
       <c r="C28" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="D28" s="2" t="n">
+        <v>54</v>
+      </c>
       <c r="E28" s="3" t="n">
-        <v>42738</v>
+        <v>42629</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="59.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="G28" s="3" t="n">
+        <v>42629</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>61</v>
+        <v>1</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>42620</v>
+        <v>42736</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="I29" s="10" t="s">
-        <v>63</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D30" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" s="3" t="n">
+        <v>42738</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="59.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="E30" s="3" t="n">
-        <v>42622</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G30" s="3" t="n">
-        <v>42623</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
+      <c r="B31" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="D31" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="E31" s="3" t="n">
+        <v>42620</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="E32" s="3" t="n">
+        <v>42622</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="3" t="n">
+        <v>42623</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E33" s="3" t="n">
         <v>42737</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
+      <c r="F33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C32" s="1" t="n">
+      <c r="B34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E32" s="3" t="n">
-        <v>42620</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="I32" s="10" t="s">
+      <c r="D34" s="2" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C33" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E33" s="3" t="n">
-        <v>42738</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C34" s="1" t="n">
-        <v>4</v>
       </c>
       <c r="E34" s="3" t="n">
         <v>42620</v>
@@ -1537,42 +1541,38 @@
         <v>10</v>
       </c>
       <c r="H34" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E35" s="3" t="n">
+        <v>42738</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D35" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="E35" s="3" t="n">
-        <v>42620</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="I35" s="9"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="C36" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E36" s="3" t="n">
         <v>42620</v>
@@ -1580,17 +1580,22 @@
       <c r="F36" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I36" s="9"/>
-    </row>
-    <row r="37" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H36" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="D37" s="2" t="n">
+        <v>30</v>
       </c>
       <c r="E37" s="3" t="n">
         <v>42620</v>
@@ -1599,18 +1604,19 @@
         <v>10</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>79</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="I37" s="9"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E38" s="3" t="n">
         <v>42620</v>
@@ -1618,16 +1624,14 @@
       <c r="F38" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>9</v>
@@ -1638,13 +1642,16 @@
       <c r="F39" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="H39" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>9</v>
@@ -1655,10 +1662,13 @@
       <c r="F40" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H40" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>84</v>
@@ -1667,61 +1677,55 @@
         <v>9</v>
       </c>
       <c r="E41" s="3" t="n">
-        <v>42629</v>
+        <v>42620</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H41" s="2" t="s">
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
-        <v>71</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>9</v>
       </c>
       <c r="E42" s="3" t="n">
-        <v>43657</v>
+        <v>42620</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H42" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="43" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
-        <v>77</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>88</v>
+        <v>57</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>9</v>
       </c>
       <c r="E43" s="3" t="n">
-        <v>43658</v>
+        <v>42629</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>9</v>
@@ -1732,102 +1736,102 @@
       <c r="F44" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H44" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E45" s="3" t="n">
+        <v>43658</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E46" s="3" t="n">
+        <v>43657</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C45" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="E45" s="3" t="n">
+      <c r="B47" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E47" s="3" t="n">
         <v>42624</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="n">
+      <c r="F47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C46" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="E46" s="3" t="n">
+      <c r="B48" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E48" s="3" t="n">
         <v>42624</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G46" s="3" t="n">
+      <c r="F48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G48" s="3" t="n">
         <v>42624</v>
       </c>
-      <c r="H46" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="n">
+      <c r="H48" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C47" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="D47" s="2" t="n">
+      <c r="B49" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="D49" s="2" t="n">
         <v>31</v>
-      </c>
-      <c r="E47" s="3" t="n">
-        <v>42622</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C48" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="E48" s="3" t="n">
-        <v>42622</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C49" s="1" t="n">
-        <v>10</v>
       </c>
       <c r="E49" s="3" t="n">
         <v>42622</v>
@@ -1836,35 +1840,35 @@
         <v>10</v>
       </c>
       <c r="H49" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E50" s="3" t="n">
+        <v>42622</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H50" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="B50" s="1" t="s">
+    <row r="51" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="C50" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="E50" s="3" t="n">
-        <v>42624</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="C51" s="1" t="n">
         <v>10</v>
@@ -1876,95 +1880,92 @@
         <v>10</v>
       </c>
       <c r="H51" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E52" s="3" t="n">
+        <v>42624</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H52" s="2" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C52" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="E52" s="3" t="n">
-        <v>42622</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C53" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E53" s="3" t="n">
+        <v>42622</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H53" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C53" s="1" t="n">
-        <v>99</v>
-      </c>
-      <c r="E53" s="3" t="n">
-        <v>43658</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H53" s="2" t="s">
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="54" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="n">
-        <v>58</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="C54" s="1" t="n">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="E54" s="3" t="n">
-        <v>42658</v>
+        <v>42622</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="C55" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="D55" s="2" t="n">
-        <v>55</v>
-      </c>
       <c r="E55" s="3" t="n">
-        <v>42629</v>
+        <v>43658</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H55" s="1" t="s">
-        <v>110</v>
+      <c r="H55" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C56" s="1" t="n">
         <v>99</v>
@@ -1976,29 +1977,35 @@
         <v>10</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>99</v>
       </c>
+      <c r="D57" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="E57" s="3" t="n">
+        <v>42629</v>
+      </c>
       <c r="F57" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H57" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H57" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>113</v>
@@ -2006,62 +2013,56 @@
       <c r="C58" s="1" t="n">
         <v>99</v>
       </c>
+      <c r="E58" s="3" t="n">
+        <v>42658</v>
+      </c>
       <c r="F58" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C59" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="E59" s="3" t="n">
-        <v>42622</v>
-      </c>
       <c r="F59" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C60" s="1" t="n">
         <v>99</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G60" s="3" t="n">
-        <v>42624</v>
+        <v>10</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I60" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C61" s="1" t="n">
         <v>99</v>
@@ -2072,117 +2073,129 @@
       <c r="F61" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H61" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
-        <v>88</v>
-      </c>
-      <c r="B62" s="11" t="s">
-        <v>122</v>
+        <v>18</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="C62" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="E62" s="3" t="n">
+      <c r="F62" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G62" s="3" t="n">
+        <v>42624</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C63" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="E63" s="3" t="n">
+        <v>42622</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C64" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="E64" s="3" t="n">
         <v>43662</v>
       </c>
-      <c r="F62" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="36.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="n">
+      <c r="F64" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C65" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="E65" s="3" t="n">
+        <v>43665</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="36.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="I63" s="1"/>
-    </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H64" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="I64" s="1"/>
-    </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H65" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="I65" s="1"/>
-    </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>130</v>
+        <v>16</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="I66" s="1"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I67" s="1"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>132</v>
@@ -2191,456 +2204,487 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="n">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I69" s="1"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="n">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I70" s="1"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" customFormat="false" ht="36.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="n">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D72" s="2" t="n">
-        <v>27</v>
-      </c>
-      <c r="E72" s="3" t="n">
-        <v>42620</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="E72" s="1"/>
       <c r="F72" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G72" s="3" t="n">
-        <v>42621</v>
-      </c>
-      <c r="H72" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H72" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="I72" s="2" t="s">
-        <v>138</v>
-      </c>
+      <c r="I72" s="1"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="n">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H73" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E73" s="3" t="n">
-        <v>43657</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H73" s="2" t="s">
-        <v>140</v>
-      </c>
+      <c r="I73" s="1"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
       <c r="I74" s="1"/>
     </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="36.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="n">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>143</v>
+        <v>53</v>
+      </c>
+      <c r="D75" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="E75" s="3" t="n">
+        <v>42620</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="G75" s="3" t="n">
+        <v>42621</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="n">
-        <v>4</v>
+        <v>74</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E76" s="1"/>
+        <v>142</v>
+      </c>
+      <c r="E76" s="3" t="n">
+        <v>43657</v>
+      </c>
       <c r="F76" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H76" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="I76" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I77" s="1"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="n">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E78" s="1"/>
+        <v>146</v>
+      </c>
       <c r="F78" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H78" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="I78" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I79" s="1"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I80" s="1"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I81" s="1"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I82" s="1"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="n">
-        <v>69</v>
+        <v>9</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E83" s="3" t="n">
-        <v>43657</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="E83" s="1"/>
       <c r="F83" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H83" s="2" t="s">
-        <v>158</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I83" s="1"/>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="n">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E84" s="3" t="n">
-        <v>43657</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="E84" s="1"/>
       <c r="F84" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H84" s="2" t="s">
-        <v>160</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I84" s="1"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>113</v>
+        <v>158</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="I85" s="1" t="s">
-        <v>162</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="I85" s="1"/>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E86" s="3" t="n">
         <v>43657</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H86" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E87" s="3" t="n">
+        <v>43657</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H88" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="87" customFormat="false" ht="48" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="n">
+      <c r="I88" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E89" s="3" t="n">
+        <v>43657</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="48" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E87" s="8" t="n">
+      <c r="B90" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E90" s="8" t="n">
         <v>42605</v>
       </c>
-      <c r="F87" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G87" s="3" t="n">
+      <c r="F90" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G90" s="3" t="n">
         <v>42605</v>
       </c>
-      <c r="H87" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="I87" s="9" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="88" s="1" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D88" s="2"/>
-      <c r="F88" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G88" s="3"/>
-    </row>
-    <row r="89" s="1" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B89" s="1" t="s">
+      <c r="H90" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="D89" s="2"/>
-      <c r="F89" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G89" s="3"/>
-    </row>
-    <row r="90" s="1" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B90" s="1" t="s">
+      <c r="I90" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="D90" s="2"/>
-      <c r="F90" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G90" s="3"/>
     </row>
     <row r="91" s="1" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>171</v>
       </c>
       <c r="D91" s="2"/>
       <c r="F91" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G91" s="3"/>
     </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" s="1" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="n">
-        <v>70</v>
+        <v>14</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E92" s="3" t="n">
-        <v>43657</v>
-      </c>
+      <c r="D92" s="2"/>
       <c r="F92" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="G92" s="3"/>
+    </row>
+    <row r="93" s="1" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="n">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="E93" s="3" t="n">
-        <v>43657</v>
-      </c>
+      <c r="D93" s="2"/>
       <c r="F93" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="G93" s="3"/>
+    </row>
+    <row r="94" s="1" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="n">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E94" s="3" t="n">
-        <v>43657</v>
-      </c>
+      <c r="D94" s="2"/>
       <c r="F94" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G94" s="3"/>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="n">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>175</v>
       </c>
       <c r="E95" s="3" t="n">
-        <v>43658</v>
+        <v>43657</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="n">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C96" s="1" t="n">
-        <v>99</v>
-      </c>
       <c r="E96" s="3" t="n">
-        <v>43665</v>
+        <v>43657</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E97" s="3" t="n">
+        <v>43657</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E98" s="3" t="n">
+        <v>43658</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I94">
+  <autoFilter ref="A1:I98">
     <filterColumn colId="5">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>

<commit_message>
Issue-99 Remove DoubleCurveSegment ... references to pegCounts
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,13 +11,13 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$98</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$94</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$I$95</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$I$81</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$I$90</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$I$57</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$I$66</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$94</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$98</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$I$95</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$I$81</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$I$90</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$I$57</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$I$66</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="183">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t xml:space="preserve">Different Curve tolerances</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is this needed</t>
   </si>
   <si>
     <t xml:space="preserve">Auto Update Curves</t>
@@ -259,7 +262,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Can JavaFX use the Mac manus</t>
+    <t xml:space="preserve">Can JavaFX use the Mac menus</t>
   </si>
   <si>
     <t xml:space="preserve">Remove unused code</t>
@@ -577,6 +580,15 @@
   </si>
   <si>
     <t xml:space="preserve">CannyTransform generate egdes needs to disable EditPixels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove DoubleCurbe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Double curves are not used now that the curves can aggressively eat neighbouring pixels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove files  that should not be tracked </t>
   </si>
 </sst>
 </file>
@@ -802,12 +814,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I98"/>
+  <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E98" activeCellId="0" sqref="E98:F98"/>
+      <selection pane="bottomLeft" activeCell="G100" activeCellId="0" sqref="G100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -986,13 +998,16 @@
       <c r="F8" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="H8" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="48" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>79</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>0</v>
@@ -1004,10 +1019,10 @@
         <v>16</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="36.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1015,7 +1030,7 @@
         <v>80</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>0</v>
@@ -1027,10 +1042,10 @@
         <v>16</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1038,7 +1053,7 @@
         <v>81</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>0</v>
@@ -1053,7 +1068,7 @@
         <v>10</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1061,7 +1076,7 @@
         <v>82</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0</v>
@@ -1073,7 +1088,7 @@
         <v>16</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1081,7 +1096,7 @@
         <v>84</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0</v>
@@ -1098,7 +1113,7 @@
         <v>86</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>0</v>
@@ -1110,7 +1125,7 @@
         <v>16</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1118,7 +1133,7 @@
         <v>87</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>0</v>
@@ -1135,7 +1150,7 @@
         <v>91</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0</v>
@@ -1147,7 +1162,7 @@
         <v>16</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1155,7 +1170,7 @@
         <v>93</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0</v>
@@ -1167,7 +1182,7 @@
         <v>16</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1175,7 +1190,7 @@
         <v>94</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>0</v>
@@ -1187,7 +1202,7 @@
         <v>10</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1195,7 +1210,7 @@
         <v>64</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>1</v>
@@ -1204,10 +1219,10 @@
         <v>42738</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1215,7 +1230,7 @@
         <v>29</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>1</v>
@@ -1227,7 +1242,7 @@
         <v>16</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I20" s="1"/>
     </row>
@@ -1236,7 +1251,7 @@
         <v>63</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>1</v>
@@ -1248,7 +1263,7 @@
         <v>10</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1256,7 +1271,7 @@
         <v>40</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>1</v>
@@ -1274,7 +1289,7 @@
         <v>42621</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1282,7 +1297,7 @@
         <v>60</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>1</v>
@@ -1294,7 +1309,7 @@
         <v>16</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="71" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1302,7 +1317,7 @@
         <v>27</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>1</v>
@@ -1317,10 +1332,10 @@
         <v>42620</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1328,7 +1343,7 @@
         <v>52</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>1</v>
@@ -1351,7 +1366,7 @@
         <v>53</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>1</v>
@@ -1374,7 +1389,7 @@
         <v>54</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>1</v>
@@ -1397,7 +1412,7 @@
         <v>55</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>1</v>
@@ -1420,7 +1435,7 @@
         <v>61</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>1</v>
@@ -1437,7 +1452,7 @@
         <v>66</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>1</v>
@@ -1446,7 +1461,7 @@
         <v>42738</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="59.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1454,13 +1469,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E31" s="3" t="n">
         <v>42620</v>
@@ -1469,10 +1484,10 @@
         <v>16</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1480,7 +1495,7 @@
         <v>41</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>2</v>
@@ -1498,7 +1513,7 @@
         <v>42623</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1506,7 +1521,7 @@
         <v>62</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>2</v>
@@ -1518,7 +1533,7 @@
         <v>10</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1526,13 +1541,13 @@
         <v>31</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>3</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E34" s="3" t="n">
         <v>42620</v>
@@ -1541,10 +1556,10 @@
         <v>10</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I34" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1552,7 +1567,7 @@
         <v>65</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>3</v>
@@ -1569,7 +1584,7 @@
         <v>32</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C36" s="1" t="n">
         <v>4</v>
@@ -1581,7 +1596,7 @@
         <v>10</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1589,7 +1604,7 @@
         <v>33</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C37" s="1" t="n">
         <v>5</v>
@@ -1604,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I37" s="9"/>
     </row>
@@ -1613,7 +1628,7 @@
         <v>34</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>8</v>
@@ -1631,7 +1646,7 @@
         <v>35</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>9</v>
@@ -1643,7 +1658,7 @@
         <v>10</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1651,7 +1666,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>9</v>
@@ -1663,7 +1678,7 @@
         <v>10</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1671,7 +1686,7 @@
         <v>36</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C41" s="1" t="n">
         <v>9</v>
@@ -1688,7 +1703,7 @@
         <v>37</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>9</v>
@@ -1705,7 +1720,7 @@
         <v>57</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>9</v>
@@ -1717,7 +1732,7 @@
         <v>10</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1725,7 +1740,7 @@
         <v>71</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>9</v>
@@ -1737,7 +1752,7 @@
         <v>10</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1745,7 +1760,7 @@
         <v>77</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>9</v>
@@ -1757,7 +1772,7 @@
         <v>10</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1765,7 +1780,7 @@
         <v>73</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>9</v>
@@ -1782,7 +1797,7 @@
         <v>50</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>10</v>
@@ -1794,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1802,7 +1817,7 @@
         <v>51</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C48" s="1" t="n">
         <v>10</v>
@@ -1817,7 +1832,7 @@
         <v>42624</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1825,7 +1840,7 @@
         <v>46</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C49" s="1" t="n">
         <v>10</v>
@@ -1840,7 +1855,7 @@
         <v>10</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1848,7 +1863,7 @@
         <v>45</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C50" s="1" t="n">
         <v>10</v>
@@ -1860,7 +1875,7 @@
         <v>10</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1868,7 +1883,7 @@
         <v>48</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C51" s="1" t="n">
         <v>10</v>
@@ -1880,7 +1895,7 @@
         <v>10</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1888,7 +1903,7 @@
         <v>49</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C52" s="1" t="n">
         <v>10</v>
@@ -1897,10 +1912,10 @@
         <v>42624</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1908,7 +1923,7 @@
         <v>47</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C53" s="1" t="n">
         <v>10</v>
@@ -1920,7 +1935,7 @@
         <v>10</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1928,7 +1943,7 @@
         <v>44</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>10</v>
@@ -1945,7 +1960,7 @@
         <v>85</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C55" s="1" t="n">
         <v>99</v>
@@ -1957,7 +1972,7 @@
         <v>10</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1965,7 +1980,7 @@
         <v>58</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C56" s="1" t="n">
         <v>99</v>
@@ -1977,7 +1992,7 @@
         <v>10</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1985,7 +2000,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>99</v>
@@ -2000,7 +2015,7 @@
         <v>10</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2008,7 +2023,7 @@
         <v>59</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C58" s="1" t="n">
         <v>99</v>
@@ -2020,7 +2035,7 @@
         <v>10</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2028,7 +2043,7 @@
         <v>21</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C59" s="1" t="n">
         <v>99</v>
@@ -2037,7 +2052,7 @@
         <v>10</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2045,7 +2060,7 @@
         <v>20</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C60" s="1" t="n">
         <v>99</v>
@@ -2054,7 +2069,7 @@
         <v>10</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2062,7 +2077,7 @@
         <v>43</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C61" s="1" t="n">
         <v>99</v>
@@ -2074,7 +2089,7 @@
         <v>10</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2082,7 +2097,7 @@
         <v>18</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C62" s="1" t="n">
         <v>99</v>
@@ -2094,10 +2109,10 @@
         <v>42624</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2105,7 +2120,7 @@
         <v>42</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C63" s="1" t="n">
         <v>99</v>
@@ -2122,7 +2137,7 @@
         <v>88</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C64" s="1" t="n">
         <v>99</v>
@@ -2134,7 +2149,7 @@
         <v>10</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2142,7 +2157,7 @@
         <v>96</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C65" s="1" t="n">
         <v>99</v>
@@ -2159,14 +2174,14 @@
         <v>5</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I66" s="1"/>
     </row>
@@ -2175,14 +2190,14 @@
         <v>26</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I67" s="1"/>
     </row>
@@ -2191,14 +2206,14 @@
         <v>11</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I68" s="1"/>
     </row>
@@ -2207,14 +2222,14 @@
         <v>25</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I69" s="1"/>
     </row>
@@ -2223,14 +2238,14 @@
         <v>24</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I70" s="1"/>
     </row>
@@ -2239,14 +2254,14 @@
         <v>23</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I71" s="1"/>
     </row>
@@ -2255,14 +2270,14 @@
         <v>3</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I72" s="1"/>
     </row>
@@ -2271,14 +2286,14 @@
         <v>7</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="I73" s="1"/>
     </row>
@@ -2287,14 +2302,14 @@
         <v>22</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I74" s="1"/>
     </row>
@@ -2303,7 +2318,7 @@
         <v>39</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D75" s="2" t="n">
         <v>27</v>
@@ -2318,10 +2333,10 @@
         <v>42621</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2329,7 +2344,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E76" s="3" t="n">
         <v>43657</v>
@@ -2338,7 +2353,7 @@
         <v>16</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2346,14 +2361,14 @@
         <v>16</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I77" s="1"/>
     </row>
@@ -2362,13 +2377,13 @@
         <v>67</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2376,14 +2391,14 @@
         <v>4</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I79" s="1"/>
     </row>
@@ -2392,14 +2407,14 @@
         <v>2</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I80" s="1"/>
     </row>
@@ -2408,14 +2423,14 @@
         <v>6</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I81" s="1"/>
     </row>
@@ -2424,14 +2439,14 @@
         <v>8</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I82" s="1"/>
     </row>
@@ -2440,14 +2455,14 @@
         <v>9</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I83" s="1"/>
     </row>
@@ -2456,14 +2471,14 @@
         <v>10</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I84" s="1"/>
     </row>
@@ -2472,14 +2487,14 @@
         <v>12</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I85" s="1"/>
     </row>
@@ -2488,7 +2503,7 @@
         <v>69</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E86" s="3" t="n">
         <v>43657</v>
@@ -2497,7 +2512,7 @@
         <v>16</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2505,7 +2520,7 @@
         <v>75</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E87" s="3" t="n">
         <v>43657</v>
@@ -2514,7 +2529,7 @@
         <v>16</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2522,17 +2537,17 @@
         <v>19</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2540,7 +2555,7 @@
         <v>68</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E89" s="3" t="n">
         <v>43657</v>
@@ -2549,7 +2564,7 @@
         <v>16</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="48" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2557,7 +2572,7 @@
         <v>28</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E90" s="8" t="n">
         <v>42605</v>
@@ -2569,10 +2584,10 @@
         <v>42605</v>
       </c>
       <c r="H90" s="9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I90" s="9" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="91" s="1" customFormat="true" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2580,7 +2595,7 @@
         <v>13</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D91" s="2"/>
       <c r="F91" s="1" t="s">
@@ -2593,7 +2608,7 @@
         <v>14</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D92" s="2"/>
       <c r="F92" s="1" t="s">
@@ -2606,7 +2621,7 @@
         <v>15</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D93" s="2"/>
       <c r="F93" s="1" t="s">
@@ -2619,7 +2634,7 @@
         <v>17</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D94" s="2"/>
       <c r="F94" s="1" t="s">
@@ -2632,7 +2647,7 @@
         <v>70</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E95" s="3" t="n">
         <v>43657</v>
@@ -2646,7 +2661,7 @@
         <v>72</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E96" s="3" t="n">
         <v>43657</v>
@@ -2660,7 +2675,7 @@
         <v>76</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E97" s="3" t="n">
         <v>43657</v>
@@ -2674,7 +2689,7 @@
         <v>78</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E98" s="3" t="n">
         <v>43658</v>
@@ -2683,8 +2698,45 @@
         <v>16</v>
       </c>
     </row>
+    <row r="99" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C99" s="1" t="n">
+        <v>-10</v>
+      </c>
+      <c r="E99" s="3" t="n">
+        <v>43670</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C100" s="1" t="n">
+        <v>-10</v>
+      </c>
+      <c r="E100" s="3" t="n">
+        <v>43670</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I98">
+  <autoFilter ref="A1:I94">
     <filterColumn colId="5">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>

<commit_message>
Issue-104 File/Save progress jumps to almost complete straight away
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,16 +11,16 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$107</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$J$101</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$94</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$98</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$95</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$81</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$90</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$57</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$66</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$107</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$101</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$94</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$98</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$95</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$81</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$90</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$57</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$66</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -915,9 +915,9 @@
   <dimension ref="A1:J107"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G107" activeCellId="0" sqref="G107"/>
+      <selection pane="bottomLeft" activeCell="G104" activeCellId="0" sqref="G104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1514,7 +1514,7 @@
       <c r="D25" s="2" t="n">
         <v>88</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" s="8" t="s">
         <v>61</v>
       </c>
       <c r="F25" s="3" t="n">
@@ -3059,7 +3059,7 @@
         <v>43671</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>17</v>
+        <v>101</v>
       </c>
       <c r="I104" s="2" t="s">
         <v>206</v>
@@ -3135,12 +3135,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J107">
+  <autoFilter ref="A1:J102">
     <filterColumn colId="6">
-      <filters>
-        <filter val=""/>
-        <filter val="OPEN"/>
-      </filters>
+      <customFilters and="true">
+        <customFilter operator="equal" val="OPEN"/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Issue-108 File/Save OK button state not correct
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="215">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -682,6 +682,12 @@
   </si>
   <si>
     <t xml:space="preserve">The main image on the left hand side is not fully shown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File/Save OK button state not correct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is because it is a dialog button and not an application button.</t>
   </si>
 </sst>
 </file>
@@ -912,12 +918,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J107"/>
+  <dimension ref="A1:J108"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G104" activeCellId="0" sqref="G104"/>
+      <selection pane="bottomLeft" activeCell="B108" activeCellId="0" sqref="A108:B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3134,6 +3140,23 @@
         <v>212</v>
       </c>
     </row>
+    <row r="108" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F108" s="3" t="n">
+        <v>43674</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I108" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J102">
     <filterColumn colId="6">

</xml_diff>

<commit_message>
Issue-116 Add timing information
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -13,16 +13,16 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$115</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$J$108</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$107</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$101</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$94</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$98</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$95</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$81</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$90</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$57</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$66</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$108</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$107</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$101</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$94</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$98</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$95</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$81</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$90</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$57</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$66</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="233">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -732,6 +732,18 @@
   </si>
   <si>
     <t xml:space="preserve">This is because it is a dialog button and not an application button.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to put some performance timing in </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generate PixelChains … possibly means chaning the defaults on CET too.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Framework.util.Timer Duration time(Runnable pRunnable) </t>
   </si>
 </sst>
 </file>
@@ -962,12 +974,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J115"/>
+  <dimension ref="A1:J116"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C109" activeCellId="0" sqref="C109:C115"/>
+      <selection pane="bottomLeft" activeCell="G116" activeCellId="0" sqref="G116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3328,6 +3340,32 @@
         <v>228</v>
       </c>
     </row>
+    <row r="116" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C116" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F116" s="3" t="n">
+        <v>43677</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I116" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="J116" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J115">
     <filterColumn colId="6">

</xml_diff>

<commit_message>
Issue-110 PixelChain make mSegments immutable
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="234">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -744,6 +744,9 @@
   </si>
   <si>
     <t xml:space="preserve">Framework.util.Timer Duration time(Runnable pRunnable) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPMD segments do not line up properly when ratio is different</t>
   </si>
 </sst>
 </file>
@@ -974,12 +977,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J116"/>
+  <dimension ref="A1:J117"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G116" activeCellId="0" sqref="G116"/>
+      <selection pane="bottomLeft" activeCell="A66" activeCellId="0" sqref="A66:B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2477,6 +2480,12 @@
       <c r="E65" s="2" t="s">
         <v>139</v>
       </c>
+      <c r="F65" s="3" t="n">
+        <v>43677</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="n">
@@ -2494,6 +2503,12 @@
       <c r="E66" s="2" t="s">
         <v>139</v>
       </c>
+      <c r="F66" s="3" t="n">
+        <v>43677</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="n">
@@ -2511,6 +2526,12 @@
       <c r="E67" s="2" t="s">
         <v>139</v>
       </c>
+      <c r="F67" s="3" t="n">
+        <v>43677</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
@@ -2528,6 +2549,12 @@
       <c r="E68" s="2" t="s">
         <v>139</v>
       </c>
+      <c r="F68" s="3" t="n">
+        <v>43677</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="n">
@@ -2545,6 +2572,12 @@
       <c r="E69" s="2" t="s">
         <v>139</v>
       </c>
+      <c r="F69" s="3" t="n">
+        <v>43677</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="n">
@@ -2562,8 +2595,14 @@
       <c r="E70" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="71" customFormat="false" ht="45.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F70" s="3" t="n">
+        <v>43677</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="n">
         <v>115</v>
       </c>
@@ -2578,6 +2617,12 @@
       </c>
       <c r="E71" s="2" t="s">
         <v>139</v>
+      </c>
+      <c r="F71" s="3" t="n">
+        <v>43677</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="I71" s="2" t="s">
         <v>157</v>
@@ -3364,6 +3409,23 @@
       </c>
       <c r="J116" s="2" t="s">
         <v>232</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C117" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F117" s="3" t="n">
+        <v>43677</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue-117 EPMD segments do not line up properly when ratio is different
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -982,7 +982,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A66" activeCellId="0" sqref="A66:B66"/>
+      <selection pane="bottomLeft" activeCell="G117" activeCellId="0" sqref="G117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3425,7 +3425,7 @@
         <v>43677</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue-112 PixelChain make mPixels final
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$115</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$115</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$108</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$107</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$101</definedName>
@@ -982,7 +982,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G117" activeCellId="0" sqref="G117"/>
+      <selection pane="bottomLeft" activeCell="A68" activeCellId="0" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2553,7 +2553,7 @@
         <v>43677</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3429,7 +3429,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J115">
+  <autoFilter ref="A1:J102">
     <filterColumn colId="6">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>

<commit_message>
Issue-113 (Part) Make mSegments in PixelChain final
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="241">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -747,6 +747,27 @@
   </si>
   <si>
     <t xml:space="preserve">EPMD segments do not line up properly when ratio is different</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ImmutableVector create addAll(ImmutableVector)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ImmutableVector create removeLastElement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PixelChain </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since PC is immutable this can be set the first time that the PC is indexed to prevent the need for it to be indexed again</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove builder.buildUnvalidatedixelChain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change PixeChain to IpixelChain in Segments and Vertexe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change Equalize defaults and Line End Shape in CET</t>
   </si>
 </sst>
 </file>
@@ -977,12 +998,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J117"/>
+  <dimension ref="A1:J123"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A68" activeCellId="0" sqref="A68"/>
+      <selection pane="bottomLeft" activeCell="G122" activeCellId="0" sqref="G122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3428,6 +3449,93 @@
         <v>17</v>
       </c>
     </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F118" s="3" t="n">
+        <v>43679</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F119" s="3" t="n">
+        <v>43679</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F120" s="3" t="n">
+        <v>43679</v>
+      </c>
+      <c r="G120" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I120" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F121" s="3" t="n">
+        <v>43679</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F122" s="3" t="n">
+        <v>43679</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F123" s="3" t="n">
+        <v>43679</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J102">
     <filterColumn colId="6">

</xml_diff>

<commit_message>
Issue-113 Make mSegments in PixelChain final
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,8 +11,9 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$115</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$J$115</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$108</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$107</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$101</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="244">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -520,6 +521,9 @@
     <t xml:space="preserve">these need to be identified from 112, 113 and 114.  e.g. replace(Vertex), replace(Segment), replace(Vertex…) … probably need a ctor with Immutable pixels, immutable vertexes immutable segments</t>
   </si>
   <si>
+    <t xml:space="preserve">DONE in PixelChainBuilder</t>
+  </si>
+  <si>
     <t xml:space="preserve">View Required</t>
   </si>
   <si>
@@ -771,6 +775,9 @@
   </si>
   <si>
     <t xml:space="preserve">curveSegment and straight segment do a lot of stuff just to implement withPosition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create PixelChain refiner</t>
   </si>
 </sst>
 </file>
@@ -1001,12 +1008,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J124"/>
+  <dimension ref="A1:J125"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A123" activeCellId="0" sqref="A123:B123"/>
+      <selection pane="bottomLeft" activeCell="B125" activeCellId="0" sqref="B125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1873,7 +1880,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
         <v>103</v>
       </c>
@@ -2399,7 +2406,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
         <v>97</v>
       </c>
@@ -2419,10 +2426,10 @@
         <v>43668</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
         <v>98</v>
       </c>
@@ -2488,7 +2495,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
         <v>109</v>
       </c>
@@ -2511,7 +2518,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="n">
         <v>110</v>
       </c>
@@ -2534,7 +2541,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="n">
         <v>111</v>
       </c>
@@ -2557,7 +2564,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
         <v>112</v>
       </c>
@@ -2580,7 +2587,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="n">
         <v>113</v>
       </c>
@@ -2600,10 +2607,10 @@
         <v>43677</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="n">
         <v>114</v>
       </c>
@@ -2623,10 +2630,10 @@
         <v>43677</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="48" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="n">
         <v>115</v>
       </c>
@@ -2646,10 +2653,13 @@
         <v>43677</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="I71" s="2" t="s">
         <v>157</v>
+      </c>
+      <c r="J71" s="2" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2657,7 +2667,7 @@
         <v>21</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C72" s="1" t="n">
         <v>22</v>
@@ -2669,7 +2679,7 @@
         <v>44</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2677,7 +2687,7 @@
         <v>20</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C73" s="1" t="n">
         <v>22</v>
@@ -2689,7 +2699,7 @@
         <v>44</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2697,7 +2707,7 @@
         <v>43</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C74" s="1" t="n">
         <v>22</v>
@@ -2712,7 +2722,7 @@
         <v>44</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2720,7 +2730,7 @@
         <v>42</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C75" s="1" t="n">
         <v>22</v>
@@ -2740,7 +2750,7 @@
         <v>65</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C76" s="1" t="n">
         <v>99</v>
@@ -2760,7 +2770,7 @@
         <v>34</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C77" s="1" t="n">
         <v>99</v>
@@ -2781,7 +2791,7 @@
         <v>18</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C78" s="1" t="n">
         <v>99</v>
@@ -2793,10 +2803,10 @@
         <v>42624</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="J78" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2804,7 +2814,7 @@
         <v>96</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C79" s="1" t="n">
         <v>99</v>
@@ -2821,14 +2831,14 @@
         <v>5</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="J80" s="1"/>
     </row>
@@ -2837,14 +2847,14 @@
         <v>26</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J81" s="1"/>
     </row>
@@ -2853,14 +2863,14 @@
         <v>11</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J82" s="1"/>
     </row>
@@ -2869,14 +2879,14 @@
         <v>25</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F83" s="1"/>
       <c r="G83" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J83" s="1"/>
     </row>
@@ -2885,14 +2895,14 @@
         <v>24</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F84" s="1"/>
       <c r="G84" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J84" s="1"/>
     </row>
@@ -2901,14 +2911,14 @@
         <v>23</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J85" s="1"/>
     </row>
@@ -2917,14 +2927,14 @@
         <v>3</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F86" s="1"/>
       <c r="G86" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J86" s="1"/>
     </row>
@@ -2933,14 +2943,14 @@
         <v>7</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="J87" s="1"/>
     </row>
@@ -2949,7 +2959,7 @@
         <v>22</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F88" s="1"/>
       <c r="G88" s="1" t="s">
@@ -2980,10 +2990,10 @@
         <v>42621</v>
       </c>
       <c r="I89" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="J89" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2991,7 +3001,7 @@
         <v>74</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F90" s="3" t="n">
         <v>43657</v>
@@ -3000,7 +3010,7 @@
         <v>12</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3008,14 +3018,14 @@
         <v>16</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F91" s="1"/>
       <c r="G91" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="J91" s="1"/>
     </row>
@@ -3024,13 +3034,13 @@
         <v>67</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3038,14 +3048,14 @@
         <v>4</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F93" s="1"/>
       <c r="G93" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="J93" s="1"/>
     </row>
@@ -3054,14 +3064,14 @@
         <v>2</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F94" s="1"/>
       <c r="G94" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="J94" s="1"/>
     </row>
@@ -3070,14 +3080,14 @@
         <v>6</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F95" s="1"/>
       <c r="G95" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="J95" s="1"/>
     </row>
@@ -3086,14 +3096,14 @@
         <v>8</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F96" s="1"/>
       <c r="G96" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="J96" s="1"/>
     </row>
@@ -3102,14 +3112,14 @@
         <v>9</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F97" s="1"/>
       <c r="G97" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="J97" s="1"/>
     </row>
@@ -3118,14 +3128,14 @@
         <v>10</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F98" s="1"/>
       <c r="G98" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="J98" s="1"/>
     </row>
@@ -3134,14 +3144,14 @@
         <v>12</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F99" s="1"/>
       <c r="G99" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="J99" s="1"/>
     </row>
@@ -3150,7 +3160,7 @@
         <v>69</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F100" s="3" t="n">
         <v>43657</v>
@@ -3159,7 +3169,7 @@
         <v>12</v>
       </c>
       <c r="I100" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3167,7 +3177,7 @@
         <v>75</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F101" s="3" t="n">
         <v>43657</v>
@@ -3176,7 +3186,7 @@
         <v>12</v>
       </c>
       <c r="I101" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3184,17 +3194,17 @@
         <v>19</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F102" s="1"/>
       <c r="G102" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3202,7 +3212,7 @@
         <v>68</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F103" s="3" t="n">
         <v>43657</v>
@@ -3211,7 +3221,7 @@
         <v>12</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="45.1" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3219,7 +3229,7 @@
         <v>28</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F104" s="10" t="n">
         <v>42605</v>
@@ -3231,10 +3241,10 @@
         <v>42605</v>
       </c>
       <c r="I104" s="7" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="J104" s="7" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3242,7 +3252,7 @@
         <v>13</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F105" s="1"/>
       <c r="G105" s="1" t="s">
@@ -3256,7 +3266,7 @@
         <v>14</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F106" s="1"/>
       <c r="G106" s="1" t="s">
@@ -3270,7 +3280,7 @@
         <v>15</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F107" s="1"/>
       <c r="G107" s="1" t="s">
@@ -3284,7 +3294,7 @@
         <v>17</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F108" s="1"/>
       <c r="G108" s="1" t="s">
@@ -3298,7 +3308,7 @@
         <v>70</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F109" s="3" t="n">
         <v>43657</v>
@@ -3312,7 +3322,7 @@
         <v>72</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F110" s="3" t="n">
         <v>43657</v>
@@ -3326,7 +3336,7 @@
         <v>76</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F111" s="3" t="n">
         <v>43657</v>
@@ -3340,7 +3350,7 @@
         <v>78</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F112" s="3" t="n">
         <v>43658</v>
@@ -3354,10 +3364,10 @@
         <v>104</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F113" s="3" t="n">
         <v>43671</v>
@@ -3366,7 +3376,7 @@
         <v>17</v>
       </c>
       <c r="I113" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="23.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3374,13 +3384,13 @@
         <v>105</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D114" s="2" t="n">
         <v>73</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F114" s="3" t="n">
         <v>43671</v>
@@ -3389,7 +3399,7 @@
         <v>44</v>
       </c>
       <c r="I114" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3397,7 +3407,7 @@
         <v>108</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F115" s="3" t="n">
         <v>43674</v>
@@ -3406,21 +3416,21 @@
         <v>17</v>
       </c>
       <c r="I115" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="n">
         <v>116</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C116" s="1" t="n">
         <v>-1</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F116" s="3" t="n">
         <v>43677</v>
@@ -3429,18 +3439,18 @@
         <v>17</v>
       </c>
       <c r="I116" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="J116" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="n">
         <v>117</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C117" s="1" t="n">
         <v>-1</v>
@@ -3457,7 +3467,7 @@
         <v>118</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F118" s="3" t="n">
         <v>43679</v>
@@ -3471,7 +3481,7 @@
         <v>119</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F119" s="3" t="n">
         <v>43679</v>
@@ -3485,7 +3495,7 @@
         <v>120</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F120" s="3" t="n">
         <v>43679</v>
@@ -3494,29 +3504,29 @@
         <v>44</v>
       </c>
       <c r="I120" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="n">
         <v>121</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F121" s="3" t="n">
         <v>43679</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="n">
         <v>122</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F122" s="3" t="n">
         <v>43679</v>
@@ -3525,12 +3535,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="n">
         <v>123</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F123" s="3" t="n">
         <v>43679</v>
@@ -3544,15 +3554,24 @@
         <v>124</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J115">
+  <autoFilter ref="A1:J124">
     <filterColumn colId="6">
-      <customFilters and="true">
-        <customFilter operator="equal" val="OPEN"/>
-      </customFilters>
+      <filters>
+        <filter val=""/>
+        <filter val="OPEN"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Issue-125 Move refinement into PixelChainBuilder
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="246">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -777,7 +777,13 @@
     <t xml:space="preserve">curveSegment and straight segment do a lot of stuff just to implement withPosition</t>
   </si>
   <si>
-    <t xml:space="preserve">Create PixelChain refiner</t>
+    <t xml:space="preserve">Move refinement into PixelChainBuilder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">de lint PixelChain and PixelChainBuilder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in particular the tolerances should be passed in rather than propogating IPMTS into these classes</t>
   </si>
 </sst>
 </file>
@@ -1008,12 +1014,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J125"/>
+  <dimension ref="A1:J126"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B125" activeCellId="0" sqref="B125"/>
+      <selection pane="bottomLeft" activeCell="I127" activeCellId="0" sqref="I127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3564,6 +3570,29 @@
       <c r="B125" s="1" t="s">
         <v>243</v>
       </c>
+      <c r="F125" s="3" t="n">
+        <v>43683</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F126" s="3" t="n">
+        <v>43683</v>
+      </c>
+      <c r="G126" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I126" s="2" t="s">
+        <v>245</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J124">

</xml_diff>

<commit_message>
Issue-130 add IJ settings to project
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,19 +11,19 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$J$115</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$108</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$107</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$101</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$94</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$98</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$95</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$81</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$90</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$57</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$66</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$115</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$108</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$107</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$101</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$94</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$98</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$95</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$81</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$90</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$57</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$66</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="250">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -784,6 +784,18 @@
   </si>
   <si>
     <t xml:space="preserve">in particular the tolerances should be passed in rather than propogating IPMTS into these classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get Lombok.config working</t>
+  </si>
+  <si>
+    <t xml:space="preserve">retire Framework not null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rename PixelChain members ending X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add IJ settings to project</t>
   </si>
 </sst>
 </file>
@@ -1014,12 +1026,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J126"/>
+  <dimension ref="A1:J130"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I127" activeCellId="0" sqref="I127"/>
+      <selection pane="bottomLeft" activeCell="B130" activeCellId="0" sqref="B130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3594,13 +3606,68 @@
         <v>245</v>
       </c>
     </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F127" s="3" t="n">
+        <v>43684</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F128" s="3" t="n">
+        <v>43684</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F129" s="3" t="n">
+        <v>43684</v>
+      </c>
+      <c r="G129" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F130" s="3" t="n">
+        <v>43684</v>
+      </c>
+      <c r="G130" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J124">
+  <autoFilter ref="A1:J102">
     <filterColumn colId="6">
-      <filters>
-        <filter val=""/>
-        <filter val="OPEN"/>
-      </filters>
+      <customFilters and="true">
+        <customFilter operator="equal" val="OPEN"/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Issue-133 Range2D runs slow
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="255">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -290,6 +290,9 @@
     <t xml:space="preserve">@NotNull different code is generated in IntelliJ to Maven hence leads to different test results</t>
   </si>
   <si>
+    <t xml:space="preserve">Usning NonNull</t>
+  </si>
+  <si>
     <t xml:space="preserve">Single application event queue</t>
   </si>
   <si>
@@ -806,6 +809,9 @@
   </si>
   <si>
     <t xml:space="preserve">Make resetInChain run faster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Range2D runs slow</t>
   </si>
 </sst>
 </file>
@@ -1036,12 +1042,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J132"/>
+  <dimension ref="A1:J133"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G132" activeCellId="0" sqref="G132"/>
+      <selection pane="bottomLeft" activeCell="A133" activeCellId="0" sqref="A133:B133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1828,10 +1834,13 @@
         <v>43662</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>82</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1839,7 +1848,7 @@
         <v>103</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>2</v>
@@ -1853,7 +1862,7 @@
         <v>65</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>99</v>
@@ -1873,7 +1882,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>99</v>
@@ -1900,7 +1909,7 @@
         <v>-99</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F36" s="3" t="n">
         <v>43670</v>
@@ -1909,7 +1918,7 @@
         <v>12</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1917,13 +1926,13 @@
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C37" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F37" s="3" t="n">
         <v>42620</v>
@@ -1932,7 +1941,7 @@
         <v>17</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1940,13 +1949,13 @@
         <v>61</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F38" s="3" t="n">
         <v>42736</v>
@@ -1955,7 +1964,7 @@
         <v>17</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1963,13 +1972,13 @@
         <v>32</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C39" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F39" s="3" t="n">
         <v>42620</v>
@@ -1978,7 +1987,7 @@
         <v>17</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1986,13 +1995,13 @@
         <v>62</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C40" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F40" s="3" t="n">
         <v>42737</v>
@@ -2001,7 +2010,7 @@
         <v>17</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2009,16 +2018,16 @@
         <v>31</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C41" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F41" s="3" t="n">
         <v>42620</v>
@@ -2027,10 +2036,10 @@
         <v>17</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J41" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2038,13 +2047,13 @@
         <v>36</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F42" s="3" t="n">
         <v>42620</v>
@@ -2058,13 +2067,13 @@
         <v>37</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F43" s="3" t="n">
         <v>42620</v>
@@ -2078,13 +2087,13 @@
         <v>57</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F44" s="3" t="n">
         <v>42629</v>
@@ -2093,7 +2102,7 @@
         <v>17</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2101,13 +2110,13 @@
         <v>58</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F45" s="3" t="n">
         <v>42658</v>
@@ -2116,7 +2125,7 @@
         <v>17</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2124,7 +2133,7 @@
         <v>56</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>2</v>
@@ -2133,7 +2142,7 @@
         <v>55</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F46" s="3" t="n">
         <v>42629</v>
@@ -2142,7 +2151,7 @@
         <v>17</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2150,13 +2159,13 @@
         <v>106</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F47" s="3" t="n">
         <v>43671</v>
@@ -2165,7 +2174,7 @@
         <v>43</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2173,13 +2182,13 @@
         <v>107</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C48" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F48" s="3" t="n">
         <v>43671</v>
@@ -2188,7 +2197,7 @@
         <v>43</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2196,16 +2205,16 @@
         <v>46</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C49" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F49" s="3" t="n">
         <v>42622</v>
@@ -2214,7 +2223,7 @@
         <v>17</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2222,19 +2231,19 @@
         <v>21</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C50" s="1" t="n">
         <v>22</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2242,19 +2251,19 @@
         <v>20</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C51" s="1" t="n">
         <v>22</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2262,13 +2271,13 @@
         <v>43</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C52" s="1" t="n">
         <v>22</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F52" s="3" t="n">
         <v>42622</v>
@@ -2277,7 +2286,7 @@
         <v>17</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2285,13 +2294,13 @@
         <v>42</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C53" s="1" t="n">
         <v>22</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F53" s="3" t="n">
         <v>42622</v>
@@ -2305,10 +2314,10 @@
         <v>104</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F54" s="3" t="n">
         <v>43671</v>
@@ -2317,7 +2326,7 @@
         <v>43</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2325,13 +2334,13 @@
         <v>105</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D55" s="2" t="n">
         <v>73</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F55" s="3" t="n">
         <v>43671</v>
@@ -2340,7 +2349,7 @@
         <v>17</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2348,7 +2357,7 @@
         <v>99</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C56" s="1" t="n">
         <v>-10</v>
@@ -2360,7 +2369,7 @@
         <v>12</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2368,7 +2377,7 @@
         <v>100</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>-10</v>
@@ -2385,7 +2394,7 @@
         <v>89</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C58" s="1" t="n">
         <v>-1</v>
@@ -2397,10 +2406,10 @@
         <v>12</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2408,7 +2417,7 @@
         <v>90</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C59" s="1" t="n">
         <v>-1</v>
@@ -2420,7 +2429,7 @@
         <v>12</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="48" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2428,7 +2437,7 @@
         <v>79</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C60" s="1" t="n">
         <v>0</v>
@@ -2440,10 +2449,10 @@
         <v>12</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="36.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2451,7 +2460,7 @@
         <v>80</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C61" s="1" t="n">
         <v>0</v>
@@ -2463,10 +2472,10 @@
         <v>12</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2474,7 +2483,7 @@
         <v>82</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C62" s="1" t="n">
         <v>0</v>
@@ -2486,7 +2495,7 @@
         <v>12</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2494,7 +2503,7 @@
         <v>86</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C63" s="1" t="n">
         <v>0</v>
@@ -2506,7 +2515,7 @@
         <v>12</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2514,7 +2523,7 @@
         <v>87</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C64" s="1" t="n">
         <v>0</v>
@@ -2531,7 +2540,7 @@
         <v>91</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C65" s="1" t="n">
         <v>0</v>
@@ -2543,7 +2552,7 @@
         <v>12</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2551,7 +2560,7 @@
         <v>93</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C66" s="1" t="n">
         <v>0</v>
@@ -2563,7 +2572,7 @@
         <v>12</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2571,7 +2580,7 @@
         <v>64</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C67" s="1" t="n">
         <v>1</v>
@@ -2583,7 +2592,7 @@
         <v>43</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2591,7 +2600,7 @@
         <v>29</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C68" s="1" t="n">
         <v>1</v>
@@ -2603,7 +2612,7 @@
         <v>12</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J68" s="1"/>
     </row>
@@ -2612,7 +2621,7 @@
         <v>40</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C69" s="1" t="n">
         <v>1</v>
@@ -2630,7 +2639,7 @@
         <v>42621</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2638,7 +2647,7 @@
         <v>60</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C70" s="1" t="n">
         <v>1</v>
@@ -2650,7 +2659,7 @@
         <v>12</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="71" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2658,7 +2667,7 @@
         <v>27</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C71" s="1" t="n">
         <v>1</v>
@@ -2673,10 +2682,10 @@
         <v>42620</v>
       </c>
       <c r="I71" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="J71" s="10" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2684,7 +2693,7 @@
         <v>52</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C72" s="1" t="n">
         <v>1</v>
@@ -2707,7 +2716,7 @@
         <v>53</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C73" s="1" t="n">
         <v>1</v>
@@ -2730,7 +2739,7 @@
         <v>54</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C74" s="1" t="n">
         <v>1</v>
@@ -2753,7 +2762,7 @@
         <v>55</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C75" s="1" t="n">
         <v>1</v>
@@ -2776,7 +2785,7 @@
         <v>66</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C76" s="1" t="n">
         <v>1</v>
@@ -2793,13 +2802,13 @@
         <v>30</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C77" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F77" s="3" t="n">
         <v>42620</v>
@@ -2808,10 +2817,10 @@
         <v>12</v>
       </c>
       <c r="I77" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J77" s="10" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2819,7 +2828,7 @@
         <v>41</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C78" s="1" t="n">
         <v>2</v>
@@ -2837,7 +2846,7 @@
         <v>42623</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2845,7 +2854,7 @@
         <v>51</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C79" s="1" t="n">
         <v>10</v>
@@ -2860,7 +2869,7 @@
         <v>42624</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2868,7 +2877,7 @@
         <v>49</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C80" s="1" t="n">
         <v>10</v>
@@ -2880,7 +2889,7 @@
         <v>43</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2888,7 +2897,7 @@
         <v>18</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C81" s="1" t="n">
         <v>99</v>
@@ -2900,10 +2909,10 @@
         <v>42624</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J81" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2911,7 +2920,7 @@
         <v>96</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C82" s="1" t="n">
         <v>99</v>
@@ -2928,14 +2937,14 @@
         <v>5</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F83" s="1"/>
       <c r="G83" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I83" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="J83" s="1"/>
     </row>
@@ -2944,14 +2953,14 @@
         <v>26</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F84" s="1"/>
       <c r="G84" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="J84" s="1"/>
     </row>
@@ -2960,14 +2969,14 @@
         <v>11</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J85" s="1"/>
     </row>
@@ -2976,14 +2985,14 @@
         <v>25</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F86" s="1"/>
       <c r="G86" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J86" s="1"/>
     </row>
@@ -2992,14 +3001,14 @@
         <v>24</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="J87" s="1"/>
     </row>
@@ -3008,14 +3017,14 @@
         <v>23</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F88" s="1"/>
       <c r="G88" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="J88" s="1"/>
     </row>
@@ -3024,14 +3033,14 @@
         <v>3</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J89" s="1"/>
     </row>
@@ -3040,14 +3049,14 @@
         <v>7</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F90" s="1"/>
       <c r="G90" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="J90" s="1"/>
     </row>
@@ -3056,14 +3065,14 @@
         <v>22</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F91" s="1"/>
       <c r="G91" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J91" s="1"/>
     </row>
@@ -3072,7 +3081,7 @@
         <v>39</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D92" s="2" t="n">
         <v>27</v>
@@ -3087,10 +3096,10 @@
         <v>42621</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="J92" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3098,7 +3107,7 @@
         <v>74</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F93" s="3" t="n">
         <v>43657</v>
@@ -3107,7 +3116,7 @@
         <v>12</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3115,14 +3124,14 @@
         <v>16</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F94" s="1"/>
       <c r="G94" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="J94" s="1"/>
     </row>
@@ -3131,13 +3140,13 @@
         <v>67</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3145,14 +3154,14 @@
         <v>4</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F96" s="1"/>
       <c r="G96" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="J96" s="1"/>
     </row>
@@ -3161,14 +3170,14 @@
         <v>2</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F97" s="1"/>
       <c r="G97" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="J97" s="1"/>
     </row>
@@ -3177,14 +3186,14 @@
         <v>6</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F98" s="1"/>
       <c r="G98" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="J98" s="1"/>
     </row>
@@ -3193,14 +3202,14 @@
         <v>8</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F99" s="1"/>
       <c r="G99" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="J99" s="1"/>
     </row>
@@ -3209,14 +3218,14 @@
         <v>9</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F100" s="1"/>
       <c r="G100" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="J100" s="1"/>
     </row>
@@ -3225,14 +3234,14 @@
         <v>10</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="J101" s="1"/>
     </row>
@@ -3241,14 +3250,14 @@
         <v>12</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F102" s="1"/>
       <c r="G102" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="J102" s="1"/>
     </row>
@@ -3257,7 +3266,7 @@
         <v>69</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F103" s="3" t="n">
         <v>43657</v>
@@ -3266,7 +3275,7 @@
         <v>12</v>
       </c>
       <c r="I103" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3274,7 +3283,7 @@
         <v>75</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F104" s="3" t="n">
         <v>43657</v>
@@ -3283,7 +3292,7 @@
         <v>12</v>
       </c>
       <c r="I104" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3291,17 +3300,17 @@
         <v>19</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F105" s="1"/>
       <c r="G105" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="J105" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3309,7 +3318,7 @@
         <v>68</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F106" s="3" t="n">
         <v>43657</v>
@@ -3318,7 +3327,7 @@
         <v>12</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="48" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3326,7 +3335,7 @@
         <v>28</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F107" s="12" t="n">
         <v>42605</v>
@@ -3338,10 +3347,10 @@
         <v>42605</v>
       </c>
       <c r="I107" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="J107" s="7" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3349,7 +3358,7 @@
         <v>13</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F108" s="1"/>
       <c r="G108" s="1" t="s">
@@ -3363,7 +3372,7 @@
         <v>14</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F109" s="1"/>
       <c r="G109" s="1" t="s">
@@ -3377,7 +3386,7 @@
         <v>15</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F110" s="1"/>
       <c r="G110" s="1" t="s">
@@ -3391,7 +3400,7 @@
         <v>17</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F111" s="1"/>
       <c r="G111" s="1" t="s">
@@ -3405,7 +3414,7 @@
         <v>70</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F112" s="3" t="n">
         <v>43657</v>
@@ -3419,7 +3428,7 @@
         <v>72</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F113" s="3" t="n">
         <v>43657</v>
@@ -3433,7 +3442,7 @@
         <v>76</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F114" s="3" t="n">
         <v>43657</v>
@@ -3447,7 +3456,7 @@
         <v>78</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F115" s="3" t="n">
         <v>43658</v>
@@ -3461,7 +3470,7 @@
         <v>108</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F116" s="3" t="n">
         <v>43674</v>
@@ -3470,7 +3479,7 @@
         <v>43</v>
       </c>
       <c r="I116" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3478,7 +3487,7 @@
         <v>117</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C117" s="1" t="n">
         <v>-1</v>
@@ -3495,7 +3504,7 @@
         <v>118</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F118" s="3" t="n">
         <v>43679</v>
@@ -3509,7 +3518,7 @@
         <v>119</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F119" s="3" t="n">
         <v>43679</v>
@@ -3523,7 +3532,7 @@
         <v>120</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F120" s="3" t="n">
         <v>43679</v>
@@ -3532,7 +3541,7 @@
         <v>17</v>
       </c>
       <c r="I120" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3540,7 +3549,7 @@
         <v>121</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F121" s="3" t="n">
         <v>43679</v>
@@ -3554,7 +3563,7 @@
         <v>122</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F122" s="3" t="n">
         <v>43679</v>
@@ -3568,7 +3577,7 @@
         <v>123</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F123" s="3" t="n">
         <v>43679</v>
@@ -3582,7 +3591,7 @@
         <v>124</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3590,7 +3599,7 @@
         <v>125</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F125" s="3" t="n">
         <v>43683</v>
@@ -3604,7 +3613,7 @@
         <v>126</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F126" s="3" t="n">
         <v>43683</v>
@@ -3613,7 +3622,7 @@
         <v>17</v>
       </c>
       <c r="I126" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3621,7 +3630,7 @@
         <v>127</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F127" s="3" t="n">
         <v>43684</v>
@@ -3635,7 +3644,7 @@
         <v>128</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F128" s="3" t="n">
         <v>43684</v>
@@ -3649,7 +3658,7 @@
         <v>129</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F129" s="3" t="n">
         <v>43684</v>
@@ -3663,7 +3672,7 @@
         <v>130</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F130" s="3" t="n">
         <v>43684</v>
@@ -3677,7 +3686,7 @@
         <v>131</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F131" s="3" t="n">
         <v>43690</v>
@@ -3686,7 +3695,7 @@
         <v>17</v>
       </c>
       <c r="I131" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3694,13 +3703,27 @@
         <v>132</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F132" s="3" t="n">
         <v>43693</v>
       </c>
       <c r="G132" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F133" s="3" t="n">
+        <v>43697</v>
+      </c>
+      <c r="G133" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue-134 Delete Pixel Chain in EPMD is slow
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="256">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -812,6 +812,9 @@
   </si>
   <si>
     <t xml:space="preserve">Range2D runs slow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete Pixel Chain in EPMD is slow</t>
   </si>
 </sst>
 </file>
@@ -1042,12 +1045,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J133"/>
+  <dimension ref="A1:J134"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A133" activeCellId="0" sqref="A133:B133"/>
+      <selection pane="bottomLeft" activeCell="G134" activeCellId="0" sqref="G134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3726,6 +3729,20 @@
         <v>43</v>
       </c>
     </row>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F134" s="3" t="n">
+        <v>43698</v>
+      </c>
+      <c r="G134" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J130">
     <filterColumn colId="6">

</xml_diff>

<commit_message>
Issue-135 Remove IPixelMapTransformSource from PixelChain
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="257">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -815,6 +815,9 @@
   </si>
   <si>
     <t xml:space="preserve">Delete Pixel Chain in EPMD is slow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove IpixelMapTransformSource fom PixelChain</t>
   </si>
 </sst>
 </file>
@@ -1045,12 +1048,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J134"/>
+  <dimension ref="A1:J135"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G134" activeCellId="0" sqref="G134"/>
+      <selection pane="bottomLeft" activeCell="A135" activeCellId="0" sqref="A135:B135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3743,6 +3746,20 @@
         <v>43</v>
       </c>
     </row>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F135" s="3" t="n">
+        <v>43699</v>
+      </c>
+      <c r="G135" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J130">
     <filterColumn colId="6">

</xml_diff>

<commit_message>
Issue-141 Centralize PixelChain changes in PixelMap
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="263">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -833,6 +833,9 @@
   </si>
   <si>
     <t xml:space="preserve">CET Generate throws error … only noticed because switched on OpenCL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PixelMap centralise all pixelChain changes.</t>
   </si>
 </sst>
 </file>
@@ -1063,12 +1066,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J140"/>
+  <dimension ref="A1:J141"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C141" activeCellId="0" sqref="C141"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="G141" activeCellId="0" sqref="G141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3815,6 +3818,20 @@
         <v>261</v>
       </c>
     </row>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="F141" s="3" t="n">
+        <v>43702</v>
+      </c>
+      <c r="G141" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J130">
     <filterColumn colId="6">

</xml_diff>

<commit_message>
Issue-147 Generated PixeclChains can not be deleted
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="269">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -845,6 +845,15 @@
   </si>
   <si>
     <t xml:space="preserve">ImmutableMap2D change set to put</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convert to curves does not delete old segments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When drawing new PC it only approximates with straight lines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generated PixeclChains can not be deleted</t>
   </si>
 </sst>
 </file>
@@ -857,13 +866,12 @@
     <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="167" formatCode="DD\-MMM"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -882,14 +890,90 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -898,12 +982,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -911,8 +1037,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -936,6 +1077,57 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -954,15 +1146,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -995,28 +1187,45 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Heading" xfId="20"/>
+    <cellStyle name="Heading 1" xfId="21"/>
+    <cellStyle name="Heading 2" xfId="22"/>
+    <cellStyle name="Text" xfId="23"/>
+    <cellStyle name="Note" xfId="24"/>
+    <cellStyle name="Footnote" xfId="25"/>
+    <cellStyle name="Hyperlink" xfId="26"/>
+    <cellStyle name="Status" xfId="27"/>
+    <cellStyle name="Good" xfId="28"/>
+    <cellStyle name="Neutral" xfId="29"/>
+    <cellStyle name="Bad" xfId="30"/>
+    <cellStyle name="Warning" xfId="31"/>
+    <cellStyle name="Error" xfId="32"/>
+    <cellStyle name="Accent" xfId="33"/>
+    <cellStyle name="Accent 1" xfId="34"/>
+    <cellStyle name="Accent 2" xfId="35"/>
+    <cellStyle name="Accent 3" xfId="36"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFF2F2F2"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0000EE"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -1024,11 +1233,11 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFF2F2F2"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1044,7 +1253,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -1075,12 +1284,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J144"/>
+  <dimension ref="A1:J147"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G142" activeCellId="0" sqref="G142"/>
+      <selection pane="bottomLeft" activeCell="A147" activeCellId="0" sqref="A147:B147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3865,6 +4074,9 @@
       <c r="F143" s="3" t="n">
         <v>43702</v>
       </c>
+      <c r="G143" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="n">
@@ -3872,6 +4084,45 @@
       </c>
       <c r="B144" s="1" t="s">
         <v>265</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F145" s="3" t="n">
+        <v>43706</v>
+      </c>
+      <c r="G145" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F146" s="3" t="n">
+        <v>43706</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F147" s="3" t="n">
+        <v>43707</v>
+      </c>
+      <c r="G147" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue-146 When drawing new PC it only approximates with straight lines
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="270">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -854,6 +854,9 @@
   </si>
   <si>
     <t xml:space="preserve">Generated PixeclChains can not be deleted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When moving in EPMD should not draw lines</t>
   </si>
 </sst>
 </file>
@@ -1284,12 +1287,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J147"/>
+  <dimension ref="A1:J148"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A147" activeCellId="0" sqref="A147:B147"/>
+      <selection pane="bottomLeft" activeCell="G146" activeCellId="0" sqref="G146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4003,6 +4006,9 @@
       <c r="B136" s="1" t="s">
         <v>257</v>
       </c>
+      <c r="F136" s="3" t="n">
+        <v>43699</v>
+      </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="n">
@@ -4011,6 +4017,9 @@
       <c r="B137" s="1" t="s">
         <v>258</v>
       </c>
+      <c r="F137" s="3" t="n">
+        <v>43699</v>
+      </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="n">
@@ -4019,6 +4028,12 @@
       <c r="B138" s="1" t="s">
         <v>259</v>
       </c>
+      <c r="F138" s="3" t="n">
+        <v>43699</v>
+      </c>
+      <c r="G138" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="n">
@@ -4027,6 +4042,9 @@
       <c r="B139" s="1" t="s">
         <v>260</v>
       </c>
+      <c r="F139" s="3" t="n">
+        <v>43699</v>
+      </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="n">
@@ -4035,6 +4053,9 @@
       <c r="B140" s="1" t="s">
         <v>261</v>
       </c>
+      <c r="F140" s="3" t="n">
+        <v>43699</v>
+      </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="n">
@@ -4085,6 +4106,9 @@
       <c r="B144" s="1" t="s">
         <v>265</v>
       </c>
+      <c r="F144" s="3" t="n">
+        <v>43702</v>
+      </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="n">
@@ -4110,6 +4134,9 @@
       <c r="F146" s="3" t="n">
         <v>43706</v>
       </c>
+      <c r="G146" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="n">
@@ -4123,6 +4150,14 @@
       </c>
       <c r="G147" s="1" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue-148 When moving in EPMD should not draw lines
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="270">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -1292,7 +1292,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G146" activeCellId="0" sqref="G146"/>
+      <selection pane="bottomLeft" activeCell="B148" activeCellId="0" sqref="B148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4159,6 +4159,12 @@
       <c r="B148" s="1" t="s">
         <v>269</v>
       </c>
+      <c r="F148" s="3" t="n">
+        <v>43707</v>
+      </c>
+      <c r="G148" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J130">

</xml_diff>

<commit_message>
Issue-153 Add show pixels checkbox to EPMD
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="276">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -832,6 +832,9 @@
     <t xml:space="preserve">Check performance of all Actions in EPMD and their draggability</t>
   </si>
   <si>
+    <t xml:space="preserve">149, 150, 151, 152</t>
+  </si>
+  <si>
     <t xml:space="preserve">CET Generate throws error … only noticed because switched on OpenCL</t>
   </si>
   <si>
@@ -857,6 +860,21 @@
   </si>
   <si>
     <t xml:space="preserve">When moving in EPMD should not draw lines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Action pixel of and off wide only reapproximates new curves with straight lines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toggle needs batch acceleration like pixel, and also approximate with curves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check clickability of delete pixelChain and the wide options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change pixelchain thickness should have a draggable option</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add show pixels checkbox to EPMD</t>
   </si>
 </sst>
 </file>
@@ -875,6 +893,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -892,29 +911,34 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
-      <sz val="24"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF333333"/>
+      <color rgb="FFCC0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -922,6 +946,36 @@
       <color rgb="FF808080"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -929,44 +983,21 @@
       <color rgb="FF0000EE"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFCC0000"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -974,6 +1005,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -982,30 +1014,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1023,6 +1031,30 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -1080,55 +1112,55 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="8" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -1197,23 +1229,23 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Heading" xfId="20"/>
-    <cellStyle name="Heading 1" xfId="21"/>
-    <cellStyle name="Heading 2" xfId="22"/>
-    <cellStyle name="Text" xfId="23"/>
-    <cellStyle name="Note" xfId="24"/>
-    <cellStyle name="Footnote" xfId="25"/>
-    <cellStyle name="Hyperlink" xfId="26"/>
-    <cellStyle name="Status" xfId="27"/>
-    <cellStyle name="Good" xfId="28"/>
-    <cellStyle name="Neutral" xfId="29"/>
-    <cellStyle name="Bad" xfId="30"/>
-    <cellStyle name="Warning" xfId="31"/>
-    <cellStyle name="Error" xfId="32"/>
-    <cellStyle name="Accent" xfId="33"/>
-    <cellStyle name="Accent 1" xfId="34"/>
-    <cellStyle name="Accent 2" xfId="35"/>
-    <cellStyle name="Accent 3" xfId="36"/>
+    <cellStyle name="Accent 1 17" xfId="20"/>
+    <cellStyle name="Accent 16" xfId="21"/>
+    <cellStyle name="Accent 2 18" xfId="22"/>
+    <cellStyle name="Accent 3 19" xfId="23"/>
+    <cellStyle name="Bad 13" xfId="24"/>
+    <cellStyle name="Error 15" xfId="25"/>
+    <cellStyle name="Footnote 8" xfId="26"/>
+    <cellStyle name="Good 11" xfId="27"/>
+    <cellStyle name="Heading 1 4" xfId="28"/>
+    <cellStyle name="Heading 2 5" xfId="29"/>
+    <cellStyle name="Heading 3" xfId="30"/>
+    <cellStyle name="Hyperlink 9" xfId="31"/>
+    <cellStyle name="Neutral 12" xfId="32"/>
+    <cellStyle name="Note 7" xfId="33"/>
+    <cellStyle name="Status 10" xfId="34"/>
+    <cellStyle name="Text 6" xfId="35"/>
+    <cellStyle name="Warning 14" xfId="36"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1287,12 +1319,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J148"/>
+  <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B148" activeCellId="0" sqref="B148"/>
+      <selection pane="bottomLeft" activeCell="A153" activeCellId="0" sqref="A153:B153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4009,6 +4041,9 @@
       <c r="F136" s="3" t="n">
         <v>43699</v>
       </c>
+      <c r="G136" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="n">
@@ -4020,6 +4055,9 @@
       <c r="F137" s="3" t="n">
         <v>43699</v>
       </c>
+      <c r="G137" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="n">
@@ -4042,8 +4080,14 @@
       <c r="B139" s="1" t="s">
         <v>260</v>
       </c>
+      <c r="C139" s="1" t="s">
+        <v>261</v>
+      </c>
       <c r="F139" s="3" t="n">
         <v>43699</v>
+      </c>
+      <c r="G139" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4051,10 +4095,13 @@
         <v>140</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F140" s="3" t="n">
         <v>43699</v>
+      </c>
+      <c r="G140" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4062,7 +4109,7 @@
         <v>141</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F141" s="3" t="n">
         <v>43702</v>
@@ -4076,7 +4123,7 @@
         <v>142</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F142" s="3" t="n">
         <v>43702</v>
@@ -4090,7 +4137,7 @@
         <v>143</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F143" s="3" t="n">
         <v>43702</v>
@@ -4104,10 +4151,13 @@
         <v>144</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F144" s="3" t="n">
         <v>43702</v>
+      </c>
+      <c r="G144" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4115,7 +4165,7 @@
         <v>145</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F145" s="3" t="n">
         <v>43706</v>
@@ -4129,7 +4179,7 @@
         <v>146</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F146" s="3" t="n">
         <v>43706</v>
@@ -4143,7 +4193,7 @@
         <v>147</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="F147" s="3" t="n">
         <v>43707</v>
@@ -4157,12 +4207,105 @@
         <v>148</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F148" s="3" t="n">
         <v>43707</v>
       </c>
       <c r="G148" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C149" s="0" t="n">
+        <v>-100</v>
+      </c>
+      <c r="D149" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="F149" s="3" t="n">
+        <v>43707</v>
+      </c>
+      <c r="G149" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C150" s="0"/>
+      <c r="D150" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="F150" s="3" t="n">
+        <v>43707</v>
+      </c>
+      <c r="G150" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="1" t="n">
+        <v>151</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C151" s="0"/>
+      <c r="D151" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="F151" s="3" t="n">
+        <v>43707</v>
+      </c>
+      <c r="G151" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C152" s="0" t="n">
+        <v>-100</v>
+      </c>
+      <c r="D152" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="F152" s="3" t="n">
+        <v>43707</v>
+      </c>
+      <c r="G152" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C153" s="0" t="n">
+        <v>-100</v>
+      </c>
+      <c r="F153" s="3" t="n">
+        <v>43707</v>
+      </c>
+      <c r="G153" s="1" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Issue-155 Change NY to Chester image
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -12,19 +12,20 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$115</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$108</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$107</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$101</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$94</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$98</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$95</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$81</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$90</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$57</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$66</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$153</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$115</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$108</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$107</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$101</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$94</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$98</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$95</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$81</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$90</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$57</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$66</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="280">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -875,6 +876,18 @@
   </si>
   <si>
     <t xml:space="preserve">Add show pixels checkbox to EPMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allow drag all on Crop view</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change NY → Chester image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run from perception directory does not work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main display does not show all of the image if it is large</t>
   </si>
 </sst>
 </file>
@@ -1319,12 +1332,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J153"/>
+  <dimension ref="A1:J157"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A153" activeCellId="0" sqref="A153:B153"/>
+      <selection pane="bottomLeft" activeCell="G157" activeCellId="0" sqref="G157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2091,7 +2104,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>88</v>
       </c>
@@ -3975,7 +3988,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="n">
         <v>132</v>
       </c>
@@ -3989,7 +4002,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="n">
         <v>133</v>
       </c>
@@ -4003,7 +4016,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="n">
         <v>134</v>
       </c>
@@ -4017,7 +4030,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="n">
         <v>135</v>
       </c>
@@ -4059,7 +4072,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="n">
         <v>138</v>
       </c>
@@ -4104,7 +4117,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="n">
         <v>141</v>
       </c>
@@ -4118,7 +4131,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="n">
         <v>142</v>
       </c>
@@ -4132,7 +4145,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="n">
         <v>143</v>
       </c>
@@ -4160,7 +4173,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="n">
         <v>145</v>
       </c>
@@ -4174,7 +4187,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="n">
         <v>146</v>
       </c>
@@ -4188,7 +4201,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="n">
         <v>147</v>
       </c>
@@ -4202,7 +4215,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="n">
         <v>148</v>
       </c>
@@ -4292,7 +4305,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="n">
         <v>153</v>
       </c>
@@ -4307,6 +4320,62 @@
       </c>
       <c r="G153" s="1" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F154" s="3" t="n">
+        <v>43711</v>
+      </c>
+      <c r="G154" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="F155" s="3" t="n">
+        <v>43711</v>
+      </c>
+      <c r="G155" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F156" s="3" t="n">
+        <v>43711</v>
+      </c>
+      <c r="G156" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="1" t="n">
+        <v>157</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F157" s="3" t="n">
+        <v>43711</v>
+      </c>
+      <c r="G157" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue-154 Allow drag all on Crop view
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -1337,7 +1337,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G157" activeCellId="0" sqref="G157"/>
+      <selection pane="bottomLeft" activeCell="G156" activeCellId="0" sqref="G156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4361,7 +4361,7 @@
         <v>43711</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Issue-158 Cannot drawString in Grafitti and removal of redundant setValue of mPreviewPicture in GenerateEdgesDialog
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -12,20 +12,21 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$153</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$115</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$108</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$107</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$101</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$94</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$98</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$95</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$81</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$90</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$57</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$66</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$153</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$115</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$108</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$107</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$101</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$94</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$98</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$95</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$81</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$90</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$57</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$66</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="282">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -887,7 +888,13 @@
     <t xml:space="preserve">run from perception directory does not work</t>
   </si>
   <si>
-    <t xml:space="preserve">Main display does not show all of the image if it is large</t>
+    <t xml:space="preserve">Main display does not show all of the image if it is large as it resizes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cannot drawString in Grafitti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement openCL for transforms</t>
   </si>
 </sst>
 </file>
@@ -1332,12 +1339,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J157"/>
+  <dimension ref="A1:J159"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G156" activeCellId="0" sqref="G156"/>
+      <selection pane="bottomLeft" activeCell="G159" activeCellId="0" sqref="G159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4322,7 +4329,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="n">
         <v>154</v>
       </c>
@@ -4336,7 +4343,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="n">
         <v>155</v>
       </c>
@@ -4350,7 +4357,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="n">
         <v>156</v>
       </c>
@@ -4375,6 +4382,34 @@
         <v>43711</v>
       </c>
       <c r="G157" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="1" t="n">
+        <v>158</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F158" s="3" t="n">
+        <v>43711</v>
+      </c>
+      <c r="G158" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F159" s="3" t="n">
+        <v>43711</v>
+      </c>
+      <c r="G159" s="1" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Issue-157 Main display does not show all of the image if it is large as it resizes (but dialogs should resize)
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$153</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
@@ -1344,7 +1344,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G159" activeCellId="0" sqref="G159"/>
+      <selection pane="bottomLeft" activeCell="B157" activeCellId="0" sqref="B157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4382,7 +4382,7 @@
         <v>43711</v>
       </c>
       <c r="G157" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4414,7 +4414,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J130">
+  <autoFilter ref="A1:J157">
     <filterColumn colId="6">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>

<commit_message>
Issue-160 When dragging sliders on GenerateEdges dialog the updatePreview was repeatedly being called
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$153</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="283">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -895,6 +895,9 @@
   </si>
   <si>
     <t xml:space="preserve">Implement openCL for transforms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When dragging sliders on GenerateEdges dialog the updatePreview was repeatedly being called</t>
   </si>
 </sst>
 </file>
@@ -1339,12 +1342,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J159"/>
+  <dimension ref="A1:J160"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B157" activeCellId="0" sqref="B157"/>
+      <selection pane="bottomLeft" activeCell="B160" activeCellId="0" sqref="B160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4413,8 +4416,22 @@
         <v>17</v>
       </c>
     </row>
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F160" s="3" t="n">
+        <v>43721</v>
+      </c>
+      <c r="G160" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J157">
+  <autoFilter ref="A1:J130">
     <filterColumn colId="6">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>

<commit_message>
Issue-161 Move expensive part of CannyEdgeDetector to OpenCL
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$153</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="284">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -898,6 +898,9 @@
   </si>
   <si>
     <t xml:space="preserve">When dragging sliders on GenerateEdges dialog the updatePreview was repeatedly being called</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move expensive part of CannyEdgeDetector to OpenCL</t>
   </si>
 </sst>
 </file>
@@ -1342,12 +1345,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J160"/>
+  <dimension ref="A1:J161"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B160" activeCellId="0" sqref="B160"/>
+      <selection pane="bottomLeft" activeCell="B161" activeCellId="0" sqref="B161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4430,8 +4433,22 @@
         <v>43</v>
       </c>
     </row>
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="1" t="n">
+        <v>161</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F161" s="3" t="n">
+        <v>43720</v>
+      </c>
+      <c r="G161" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J130">
+  <autoFilter ref="A1:J157">
     <filterColumn colId="6">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>

<commit_message>
Issue-162 Fix enabled status of generate CET button
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$153</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="286">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -840,6 +840,9 @@
     <t xml:space="preserve">CET Generate throws error … only noticed because switched on OpenCL</t>
   </si>
   <si>
+    <t xml:space="preserve">fixed in 161</t>
+  </si>
+  <si>
     <t xml:space="preserve">PixelMap centralise all pixelChain changes.</t>
   </si>
   <si>
@@ -901,6 +904,9 @@
   </si>
   <si>
     <t xml:space="preserve">Move expensive part of CannyEdgeDetector to OpenCL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fix enabled status of generate CET button</t>
   </si>
 </sst>
 </file>
@@ -1345,12 +1351,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J161"/>
+  <dimension ref="A1:J162"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B161" activeCellId="0" sqref="B161"/>
+      <selection pane="bottomLeft" activeCell="B162" activeCellId="0" sqref="B162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4127,7 +4133,10 @@
         <v>43699</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
+      </c>
+      <c r="J140" s="2" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4135,7 +4144,7 @@
         <v>141</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F141" s="3" t="n">
         <v>43702</v>
@@ -4149,7 +4158,7 @@
         <v>142</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F142" s="3" t="n">
         <v>43702</v>
@@ -4163,7 +4172,7 @@
         <v>143</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F143" s="3" t="n">
         <v>43702</v>
@@ -4177,7 +4186,7 @@
         <v>144</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F144" s="3" t="n">
         <v>43702</v>
@@ -4191,7 +4200,7 @@
         <v>145</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F145" s="3" t="n">
         <v>43706</v>
@@ -4205,7 +4214,7 @@
         <v>146</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="F146" s="3" t="n">
         <v>43706</v>
@@ -4219,7 +4228,7 @@
         <v>147</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F147" s="3" t="n">
         <v>43707</v>
@@ -4233,7 +4242,7 @@
         <v>148</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F148" s="3" t="n">
         <v>43707</v>
@@ -4247,7 +4256,7 @@
         <v>149</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C149" s="0" t="n">
         <v>-100</v>
@@ -4267,7 +4276,7 @@
         <v>150</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C150" s="0"/>
       <c r="D150" s="1" t="n">
@@ -4285,7 +4294,7 @@
         <v>151</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C151" s="0"/>
       <c r="D151" s="1" t="n">
@@ -4303,7 +4312,7 @@
         <v>152</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C152" s="0" t="n">
         <v>-100</v>
@@ -4323,7 +4332,7 @@
         <v>153</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C153" s="0" t="n">
         <v>-100</v>
@@ -4340,7 +4349,7 @@
         <v>154</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F154" s="3" t="n">
         <v>43711</v>
@@ -4354,7 +4363,7 @@
         <v>155</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F155" s="3" t="n">
         <v>43711</v>
@@ -4368,7 +4377,7 @@
         <v>156</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="F156" s="3" t="n">
         <v>43711</v>
@@ -4382,7 +4391,7 @@
         <v>157</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F157" s="3" t="n">
         <v>43711</v>
@@ -4396,7 +4405,7 @@
         <v>158</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="F158" s="3" t="n">
         <v>43711</v>
@@ -4410,7 +4419,7 @@
         <v>159</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F159" s="3" t="n">
         <v>43711</v>
@@ -4424,7 +4433,7 @@
         <v>160</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F160" s="3" t="n">
         <v>43721</v>
@@ -4438,7 +4447,7 @@
         <v>161</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F161" s="3" t="n">
         <v>43720</v>
@@ -4447,8 +4456,22 @@
         <v>43</v>
       </c>
     </row>
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F162" s="3" t="n">
+        <v>43727</v>
+      </c>
+      <c r="G162" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J157">
+  <autoFilter ref="A1:J130">
     <filterColumn colId="6">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>

<commit_message>
Issue-36 Recently added files list
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$153</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
@@ -1354,9 +1354,9 @@
   <dimension ref="A1:J162"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B162" activeCellId="0" sqref="B162"/>
+      <selection pane="bottomLeft" activeCell="G42" activeCellId="0" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2368,7 +2368,7 @@
         <v>42620</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4471,7 +4471,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J130">
+  <autoFilter ref="A1:J157">
     <filterColumn colId="6">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>

<commit_message>
Issue-163 EPMD throws exception when closing with large changes
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="289">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -907,6 +907,15 @@
   </si>
   <si>
     <t xml:space="preserve">Fix enabled status of generate CET button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPMD throws exception when closing with large changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPMD does not disable close buttons when performing long action e.g. large wide delete pixel chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check that delete very wide on EPMD uses parallel for initial search</t>
   </si>
 </sst>
 </file>
@@ -1351,12 +1360,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J162"/>
+  <dimension ref="A1:J165"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G42" activeCellId="0" sqref="G42"/>
+      <selection pane="bottomLeft" activeCell="G163" activeCellId="0" sqref="G163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4470,6 +4479,48 @@
         <v>43</v>
       </c>
     </row>
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="1" t="n">
+        <v>163</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F163" s="3" t="n">
+        <v>43736</v>
+      </c>
+      <c r="G163" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="1" t="n">
+        <v>164</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="F164" s="3" t="n">
+        <v>43736</v>
+      </c>
+      <c r="G164" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="1" t="n">
+        <v>165</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F165" s="3" t="n">
+        <v>43736</v>
+      </c>
+      <c r="G165" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J157">
     <filterColumn colId="6">

</xml_diff>

<commit_message>
Issue-164 EPMD does not disable close buttons when performing long action e.g. large wide delete pixel chain
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$153</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
@@ -1365,7 +1365,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G163" activeCellId="0" sqref="G163"/>
+      <selection pane="bottomLeft" activeCell="G164" activeCellId="0" sqref="G164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4504,7 +4504,7 @@
         <v>43736</v>
       </c>
       <c r="G164" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4522,7 +4522,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J157">
+  <autoFilter ref="A1:J130">
     <filterColumn colId="6">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>

<commit_message>
Issue-165 Make delete very wide on EPMD uses parallel for initial search
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$153</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
@@ -915,7 +915,7 @@
     <t xml:space="preserve">EPMD does not disable close buttons when performing long action e.g. large wide delete pixel chain</t>
   </si>
   <si>
-    <t xml:space="preserve">Check that delete very wide on EPMD uses parallel for initial search</t>
+    <t xml:space="preserve">Make delete very wide on EPMD uses parallel for initial search</t>
   </si>
 </sst>
 </file>
@@ -1365,7 +1365,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G164" activeCellId="0" sqref="G164"/>
+      <selection pane="bottomLeft" activeCell="G165" activeCellId="0" sqref="G165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4518,11 +4518,11 @@
         <v>43736</v>
       </c>
       <c r="G165" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J130">
+  <autoFilter ref="A1:J157">
     <filterColumn colId="6">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>

<commit_message>
Issue-163 EPMD throws exception when closing with large changes ImmutableNode no longer used recursion to getMaster, this means that the stack overflow issue is avoided.
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="294">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -912,10 +912,25 @@
     <t xml:space="preserve">EPMD throws exception when closing with large changes</t>
   </si>
   <si>
+    <t xml:space="preserve">This was caused by a stack overflow error on the ImmutableNode</t>
+  </si>
+  <si>
     <t xml:space="preserve">EPMD does not disable close buttons when performing long action e.g. large wide delete pixel chain</t>
   </si>
   <si>
     <t xml:space="preserve">Make delete very wide on EPMD uses parallel for initial search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevent EPMD closing when there is still a long running action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EditPixelMap improve speed of drag options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prevent closure of EditPixelMap dialog before the current long running operation has finished</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improve Range2D parallel performance</t>
   </si>
 </sst>
 </file>
@@ -1360,12 +1375,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J165"/>
+  <dimension ref="A1:J169"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G165" activeCellId="0" sqref="G165"/>
+      <selection pane="bottomLeft" activeCell="A169" activeCellId="0" sqref="A169:B169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4479,7 +4494,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="n">
         <v>163</v>
       </c>
@@ -4491,6 +4506,9 @@
       </c>
       <c r="G163" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="I163" s="2" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4498,7 +4516,7 @@
         <v>164</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="F164" s="3" t="n">
         <v>43736</v>
@@ -4512,12 +4530,68 @@
         <v>165</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="F165" s="3" t="n">
         <v>43736</v>
       </c>
       <c r="G165" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="1" t="n">
+        <v>166</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F166" s="3" t="n">
+        <v>43738</v>
+      </c>
+      <c r="G166" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F167" s="3" t="n">
+        <v>43739</v>
+      </c>
+      <c r="G167" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="F168" s="3" t="n">
+        <v>43739</v>
+      </c>
+      <c r="G168" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="1" t="n">
+        <v>169</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F169" s="3" t="n">
+        <v>43739</v>
+      </c>
+      <c r="G169" s="1" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Issue-170 Should be able to see the cursor when performing dragging operations in EPMD
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$153</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="295">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -931,6 +931,9 @@
   </si>
   <si>
     <t xml:space="preserve">Improve Range2D parallel performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should be able to see the cursor when performing dragging operations in EPMD</t>
   </si>
 </sst>
 </file>
@@ -1375,12 +1378,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J169"/>
+  <dimension ref="A1:J170"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A169" activeCellId="0" sqref="A169:B169"/>
+      <selection pane="bottomLeft" activeCell="A170" activeCellId="0" sqref="A170:B170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4595,8 +4598,22 @@
         <v>43</v>
       </c>
     </row>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F170" s="3" t="n">
+        <v>43739</v>
+      </c>
+      <c r="G170" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J157">
+  <autoFilter ref="A1:J130">
     <filterColumn colId="6">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>

<commit_message>
Issue-171 Should be able to delete pixel chain with a click in EPMD
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$153</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="296">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -934,6 +934,9 @@
   </si>
   <si>
     <t xml:space="preserve">Should be able to see the cursor when performing dragging operations in EPMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should be able to delete pixel chain with a click in EPMD</t>
   </si>
 </sst>
 </file>
@@ -1378,12 +1381,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J170"/>
+  <dimension ref="A1:J171"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A170" activeCellId="0" sqref="A170:B170"/>
+      <selection pane="bottomLeft" activeCell="A171" activeCellId="0" sqref="A171:B171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4612,8 +4615,22 @@
         <v>43</v>
       </c>
     </row>
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="1" t="n">
+        <v>171</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="F171" s="3" t="n">
+        <v>43740</v>
+      </c>
+      <c r="G171" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J130">
+  <autoFilter ref="A1:J157">
     <filterColumn colId="6">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>

<commit_message>
Issue-173 Add sample files
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$153</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="299">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -937,6 +937,15 @@
   </si>
   <si>
     <t xml:space="preserve">Should be able to delete pixel chain with a click in EPMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable File extenstions for transforms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add sample files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make runnable from GitHub … include OpenFX stuff in here</t>
   </si>
 </sst>
 </file>
@@ -1381,12 +1390,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J171"/>
+  <dimension ref="A1:J174"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A157" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A171" activeCellId="0" sqref="A171:B171"/>
+      <selection pane="bottomLeft" activeCell="B174" activeCellId="0" sqref="B174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4629,8 +4638,50 @@
         <v>43</v>
       </c>
     </row>
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="1" t="n">
+        <v>172</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="F172" s="3" t="n">
+        <v>43830</v>
+      </c>
+      <c r="G172" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="F173" s="3" t="n">
+        <v>43830</v>
+      </c>
+      <c r="G173" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="1" t="n">
+        <v>174</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F174" s="3" t="n">
+        <v>43830</v>
+      </c>
+      <c r="G174" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J157">
+  <autoFilter ref="A1:J130">
     <filterColumn colId="6">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>

<commit_message>
Issue-179 Canny Edge changes to default sizes
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$153</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="304">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -946,6 +946,21 @@
   </si>
   <si>
     <t xml:space="preserve">Make runnable from GitHub … include OpenFX stuff in here</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File exit needs to be implemented</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On Output need to have original size button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On Output need to have fixed aspect option (enter x fixes y etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On Output should have scale option</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canny Edge changes to default sizes</t>
   </si>
 </sst>
 </file>
@@ -1390,12 +1405,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J174"/>
+  <dimension ref="A1:J179"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A157" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B174" activeCellId="0" sqref="B174"/>
+      <selection pane="bottomLeft" activeCell="A179" activeCellId="0" sqref="A179:B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4680,8 +4695,78 @@
         <v>17</v>
       </c>
     </row>
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="F175" s="3" t="n">
+        <v>43823</v>
+      </c>
+      <c r="G175" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="1" t="n">
+        <v>176</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F176" s="3" t="n">
+        <v>43823</v>
+      </c>
+      <c r="G176" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="1" t="n">
+        <v>177</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F177" s="3" t="n">
+        <v>43823</v>
+      </c>
+      <c r="G177" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="1" t="n">
+        <v>178</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F178" s="3" t="n">
+        <v>43823</v>
+      </c>
+      <c r="G178" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="1" t="n">
+        <v>179</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F179" s="3" t="n">
+        <v>43823</v>
+      </c>
+      <c r="G179" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J130">
+  <autoFilter ref="A1:J157">
     <filterColumn colId="6">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>

<commit_message>
Issue-180 ImageOrganizer failing to build
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$153</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="305">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -961,6 +961,9 @@
   </si>
   <si>
     <t xml:space="preserve">Canny Edge changes to default sizes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ImageOrganizer failing to build</t>
   </si>
 </sst>
 </file>
@@ -1405,12 +1408,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J179"/>
+  <dimension ref="A1:J180"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A157" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A179" activeCellId="0" sqref="A179:B179"/>
+      <selection pane="bottomLeft" activeCell="B180" activeCellId="0" sqref="B180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4765,8 +4768,22 @@
         <v>43</v>
       </c>
     </row>
+    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F180" s="3" t="n">
+        <v>43830</v>
+      </c>
+      <c r="G180" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J157">
+  <autoFilter ref="A1:J130">
     <filterColumn colId="6">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>

<commit_message>
Issue-181 PixelChainBuilder needs to filter out candidate curve segments where the curve midpoint is not near any of the pixels.  And fix to SegmentBase getStartIndex.
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$153</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="306">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -964,6 +964,9 @@
   </si>
   <si>
     <t xml:space="preserve">ImageOrganizer failing to build</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PixelChainBuilder needs to filter out candidate curve segments where the curve midpoint is not near any of the pixels </t>
   </si>
 </sst>
 </file>
@@ -1408,12 +1411,12 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J180"/>
+  <dimension ref="A1:J181"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A157" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B180" activeCellId="0" sqref="B180"/>
+      <selection pane="bottomLeft" activeCell="B181" activeCellId="0" sqref="B181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4723,7 +4726,7 @@
         <v>43823</v>
       </c>
       <c r="G176" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4782,8 +4785,22 @@
         <v>43</v>
       </c>
     </row>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="1" t="n">
+        <v>181</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="F181" s="3" t="n">
+        <v>43830</v>
+      </c>
+      <c r="G181" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J130">
+  <autoFilter ref="A1:J157">
     <filterColumn colId="6">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>

<commit_message>
Issue-189 When leaving EPMD pixelMap is not being updated in CET.
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$153</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="310">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -978,7 +978,7 @@
     <t xml:space="preserve">PictureView should not delegate the creation of the drag delta to PictureControl</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
+    <t xml:space="preserve">When leaving EPMD pixelMap is not being updated in CET.</t>
   </si>
 </sst>
 </file>
@@ -1428,7 +1428,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B195" activeCellId="0" sqref="B195"/>
+      <selection pane="bottomLeft" activeCell="B189" activeCellId="0" sqref="B189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4913,6 +4913,12 @@
       <c r="B189" s="1" t="s">
         <v>309</v>
       </c>
+      <c r="F189" s="3" t="n">
+        <v>43923</v>
+      </c>
+      <c r="G189" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4924,7 +4930,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:J157">
+  <autoFilter ref="A1:J130">
     <filterColumn colId="6">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>

<commit_message>
Issue-190 Key press throwing exception in EPMD after Immutable added.
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$153</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="312">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -978,7 +978,13 @@
     <t xml:space="preserve">PictureView should not delegate the creation of the drag delta to PictureControl</t>
   </si>
   <si>
+    <t xml:space="preserve">Disagree … PictureView is a JavaFX facing component and so should be devoid of processing to make it easy to implement in other front end systems.</t>
+  </si>
+  <si>
     <t xml:space="preserve">When leaving EPMD pixelMap is not being updated in CET.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key press throwing exception in EPMD after Immutable added</t>
   </si>
 </sst>
 </file>
@@ -987,9 +993,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY;@"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
-    <numFmt numFmtId="167" formatCode="DD\-MMM"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="167" formatCode="dd\-mmm"/>
   </numFmts>
   <fonts count="17">
     <font>
@@ -1428,10 +1434,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B189" activeCellId="0" sqref="B189"/>
+      <selection pane="bottomLeft" activeCell="A190" activeCellId="0" sqref="A190:B190"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.5"/>
@@ -1443,7 +1449,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="16.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="42.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="9.16"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="1" width="9.16"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4892,7 +4898,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="n">
         <v>188</v>
       </c>
@@ -4903,7 +4909,10 @@
         <v>43919</v>
       </c>
       <c r="G188" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
+      </c>
+      <c r="I188" s="2" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4911,12 +4920,26 @@
         <v>189</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="F189" s="3" t="n">
         <v>43923</v>
       </c>
       <c r="G189" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="1" t="n">
+        <v>190</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F190" s="3" t="n">
+        <v>43928</v>
+      </c>
+      <c r="G190" s="1" t="s">
         <v>43</v>
       </c>
     </row>
@@ -4930,7 +4953,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:J130">
+  <autoFilter ref="A1:J157">
     <filterColumn colId="6">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>

<commit_message>
Issue-191 in EPMD use the shift key to change between move mode and pixel mode.
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -12,21 +12,22 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$153</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$115</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$108</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$107</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$101</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$94</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$98</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$95</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$81</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$90</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$57</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$66</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$192</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$153</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$115</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$108</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$107</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$101</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$94</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$98</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$95</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$81</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$90</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$57</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$66</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="316">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -985,6 +986,18 @@
   </si>
   <si>
     <t xml:space="preserve">Key press throwing exception in EPMD after Immutable added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in EPMD use the shift key to change between move mode and pixel mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in EPMD change the view to remove the concertina as this no longer drives the move/pixel view and remove the key mapping P/M that switches between them.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in EPMD use scroll wheel to change zoom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in EPMD stop the panning from getting stuck</t>
   </si>
 </sst>
 </file>
@@ -1432,9 +1445,9 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A190" activeCellId="0" sqref="A190:B190"/>
+      <selection pane="bottomLeft" activeCell="A191" activeCellId="0" sqref="A191:B191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2429,7 +2442,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
         <v>36</v>
       </c>
@@ -4200,7 +4213,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="n">
         <v>140</v>
       </c>
@@ -4464,7 +4477,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="n">
         <v>157</v>
       </c>
@@ -4478,7 +4491,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="n">
         <v>158</v>
       </c>
@@ -4506,7 +4519,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="n">
         <v>160</v>
       </c>
@@ -4520,7 +4533,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="n">
         <v>161</v>
       </c>
@@ -4534,7 +4547,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="n">
         <v>162</v>
       </c>
@@ -4548,7 +4561,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="n">
         <v>163</v>
       </c>
@@ -4565,7 +4578,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="n">
         <v>164</v>
       </c>
@@ -4579,7 +4592,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="n">
         <v>165</v>
       </c>
@@ -4593,7 +4606,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="n">
         <v>166</v>
       </c>
@@ -4607,7 +4620,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="n">
         <v>167</v>
       </c>
@@ -4621,7 +4634,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="n">
         <v>168</v>
       </c>
@@ -4635,7 +4648,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="n">
         <v>169</v>
       </c>
@@ -4649,7 +4662,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="n">
         <v>170</v>
       </c>
@@ -4663,7 +4676,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="n">
         <v>171</v>
       </c>
@@ -4677,7 +4690,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="n">
         <v>172</v>
       </c>
@@ -4691,7 +4704,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="n">
         <v>173</v>
       </c>
@@ -4733,7 +4746,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="n">
         <v>176</v>
       </c>
@@ -4775,7 +4788,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="n">
         <v>179</v>
       </c>
@@ -4789,7 +4802,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="n">
         <v>180</v>
       </c>
@@ -4803,7 +4816,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="n">
         <v>181</v>
       </c>
@@ -4859,7 +4872,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="n">
         <v>185</v>
       </c>
@@ -4873,7 +4886,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="n">
         <v>186</v>
       </c>
@@ -4884,7 +4897,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="n">
         <v>187</v>
       </c>
@@ -4898,7 +4911,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="36.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="n">
         <v>188</v>
       </c>
@@ -4915,7 +4928,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="n">
         <v>189</v>
       </c>
@@ -4929,7 +4942,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="n">
         <v>190</v>
       </c>
@@ -4941,6 +4954,62 @@
       </c>
       <c r="G190" s="1" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="1" t="n">
+        <v>191</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="F191" s="3" t="n">
+        <v>43928</v>
+      </c>
+      <c r="G191" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="F192" s="3" t="n">
+        <v>43928</v>
+      </c>
+      <c r="G192" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="1" t="n">
+        <v>193</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F193" s="3" t="n">
+        <v>43929</v>
+      </c>
+      <c r="G193" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="1" t="n">
+        <v>194</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="F194" s="3" t="n">
+        <v>43929</v>
+      </c>
+      <c r="G194" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Issue-192 in EPMD change the view to remove the concertina as this no longer drives the move/pixel view and remove the key mapping P/M that switches between them.
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$192</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$192</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$153</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="317">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -998,6 +998,9 @@
   </si>
   <si>
     <t xml:space="preserve">in EPMD stop the panning from getting stuck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPMD undo/redo/cancel issues … it is not working properly</t>
   </si>
 </sst>
 </file>
@@ -1447,7 +1450,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A191" activeCellId="0" sqref="A191:B191"/>
+      <selection pane="bottomLeft" activeCell="A192" activeCellId="0" sqref="A192:B192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4981,7 +4984,7 @@
         <v>43928</v>
       </c>
       <c r="G192" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5009,6 +5012,20 @@
         <v>43929</v>
       </c>
       <c r="G194" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="1" t="n">
+        <v>195</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="F195" s="3" t="n">
+        <v>43929</v>
+      </c>
+      <c r="G195" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5022,7 +5039,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:J157">
+  <autoFilter ref="A1:J192">
     <filterColumn colId="6">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>

<commit_message>
Issue-196 There is a problem with removePixelChian and immutability (or not) of PixelMap that has led to a hack in EPMD which can now be removed.
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="321">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -1001,6 +1001,18 @@
   </si>
   <si>
     <t xml:space="preserve">EPMD undo/redo/cancel issues … it is not working properly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is a problem with removePixelChian and immutability (or not) of PixelMap that has led to a hack in EPMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move the undo handling from CET to EPMD … this needs to prevent the generation of a new EPMD too.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change LinkedList in PixelMap to an immutable List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">see marker for Issue 196 in index(PixelChain, Isegment boolean</t>
   </si>
 </sst>
 </file>
@@ -1447,10 +1459,10 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A192" activeCellId="0" sqref="A192:B192"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="I198" activeCellId="0" sqref="I198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5026,7 +5038,52 @@
         <v>43929</v>
       </c>
       <c r="G195" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="1" t="n">
+        <v>196</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F196" s="3" t="n">
+        <v>43930</v>
+      </c>
+      <c r="G196" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="1" t="n">
+        <v>197</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="F197" s="3" t="n">
+        <v>43931</v>
+      </c>
+      <c r="G197" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="1" t="n">
+        <v>198</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F198" s="3" t="n">
+        <v>43931</v>
+      </c>
+      <c r="G198" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I198" s="2" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Issue-193 in EPMD use scroll wheel to change zoom
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -1459,10 +1459,10 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I198" activeCellId="0" sqref="I198"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B193" activeCellId="0" sqref="B193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5010,7 +5010,7 @@
         <v>43929</v>
       </c>
       <c r="G193" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5052,7 +5052,7 @@
         <v>43930</v>
       </c>
       <c r="G196" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Issue-199 Need to prevent the Savepoint error
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="323">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -1013,6 +1013,12 @@
   </si>
   <si>
     <t xml:space="preserve">see marker for Issue 196 in index(PixelChain, Isegment boolean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to prevent the Savepoint error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seems to be when you ctrl-z when the EPMD is busy</t>
   </si>
 </sst>
 </file>
@@ -1460,9 +1466,9 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B193" activeCellId="0" sqref="B193"/>
+      <selection pane="bottomLeft" activeCell="G194" activeCellId="0" sqref="G194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5024,7 +5030,7 @@
         <v>43929</v>
       </c>
       <c r="G194" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5084,6 +5090,23 @@
       </c>
       <c r="I198" s="2" t="s">
         <v>320</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="1" t="n">
+        <v>199</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="F199" s="3" t="n">
+        <v>43931</v>
+      </c>
+      <c r="G199" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I199" s="2" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Issue-203 need to make change pixel chain thickness draggable
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="330">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -1019,6 +1019,27 @@
   </si>
   <si>
     <t xml:space="preserve">seems to be when you ctrl-z when the EPMD is busy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Put in undo redo for CET editPixels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove interface Doable and convertToRuntimeException from DialogView to somewhere more generic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">there seems to be a more generic problem with undo redo for transforms … check 200 works </t>
+  </si>
+  <si>
+    <t xml:space="preserve">need to make change pixel chain thickness draggable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slider bar on zoom or buttons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">move control validation in EPMD to the generic validator based on the container</t>
+  </si>
+  <si>
+    <t xml:space="preserve">move show graffiti in EPMD to above show Curves</t>
   </si>
 </sst>
 </file>
@@ -1468,7 +1489,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G194" activeCellId="0" sqref="G194"/>
+      <selection pane="bottomLeft" activeCell="B203" activeCellId="0" sqref="B203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5072,7 +5093,7 @@
         <v>43931</v>
       </c>
       <c r="G197" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5103,10 +5124,108 @@
         <v>43931</v>
       </c>
       <c r="G199" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="I199" s="2" t="s">
         <v>322</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="F200" s="3" t="n">
+        <v>43932</v>
+      </c>
+      <c r="G200" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="F201" s="3" t="n">
+        <v>43932</v>
+      </c>
+      <c r="G201" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="1" t="n">
+        <v>202</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="F202" s="3" t="n">
+        <v>43932</v>
+      </c>
+      <c r="G202" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="1" t="n">
+        <v>203</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F203" s="3" t="n">
+        <v>43932</v>
+      </c>
+      <c r="G203" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="1" t="n">
+        <v>204</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F204" s="3" t="n">
+        <v>43932</v>
+      </c>
+      <c r="G204" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="F205" s="3" t="n">
+        <v>43933</v>
+      </c>
+      <c r="G205" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="F206" s="3" t="n">
+        <v>43933</v>
+      </c>
+      <c r="G206" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Issue-206 move show graffiti in EPMD to above show Curves
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -1489,7 +1489,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B203" activeCellId="0" sqref="B203"/>
+      <selection pane="bottomLeft" activeCell="B178" activeCellId="0" sqref="B178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5225,7 +5225,7 @@
         <v>43933</v>
       </c>
       <c r="G206" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Issue-205 move control validation in EPMD to the generic validator based on the container
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -1489,7 +1489,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B178" activeCellId="0" sqref="B178"/>
+      <selection pane="bottomLeft" activeCell="B205" activeCellId="0" sqref="B205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5211,7 +5211,7 @@
         <v>43933</v>
       </c>
       <c r="G205" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Issue-201 Remove interface Doable and convertToRuntimeException from DialogView to somewhere more generic
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -1489,7 +1489,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B205" activeCellId="0" sqref="B205"/>
+      <selection pane="bottomLeft" activeCell="G201" activeCellId="0" sqref="G201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5155,7 +5155,7 @@
         <v>43932</v>
       </c>
       <c r="G201" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Issue-198 Change LinkedList in PixelMap to an immutable List And fixing a few inspection errors
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$192</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$192</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$153</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
@@ -1027,7 +1027,7 @@
     <t xml:space="preserve">Remove interface Doable and convertToRuntimeException from DialogView to somewhere more generic</t>
   </si>
   <si>
-    <t xml:space="preserve">there seems to be a more generic problem with undo redo for transforms … check 200 works </t>
+    <t xml:space="preserve">there seems to be a more generic problem with undo redo for transforms … check Issue 200 works </t>
   </si>
   <si>
     <t xml:space="preserve">need to make change pixel chain thickness draggable</t>
@@ -1489,7 +1489,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G201" activeCellId="0" sqref="G201"/>
+      <selection pane="bottomLeft" activeCell="G198" activeCellId="0" sqref="G198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5107,7 +5107,7 @@
         <v>43931</v>
       </c>
       <c r="G198" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="I198" s="2" t="s">
         <v>320</v>
@@ -5238,7 +5238,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:J192">
+  <autoFilter ref="A1:J157">
     <filterColumn colId="6">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>

<commit_message>
Issue-207 Better layout for zoomIn/Out on EPMD
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$192</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$192</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$153</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="333">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -1040,6 +1040,15 @@
   </si>
   <si>
     <t xml:space="preserve">move show graffiti in EPMD to above show Curves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Better layout for zoomIn/Out on EPMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should have Hflow Containter etc to support 207</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of images for image buttons.</t>
   </si>
 </sst>
 </file>
@@ -1487,9 +1496,9 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G198" activeCellId="0" sqref="G198"/>
+      <selection pane="bottomLeft" activeCell="A207" activeCellId="0" sqref="A207:B207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5197,7 +5206,7 @@
         <v>43932</v>
       </c>
       <c r="G204" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5226,6 +5235,48 @@
       </c>
       <c r="G206" s="1" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="1" t="n">
+        <v>207</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="F207" s="3" t="n">
+        <v>43934</v>
+      </c>
+      <c r="G207" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="1" t="n">
+        <v>208</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="F208" s="3" t="n">
+        <v>43934</v>
+      </c>
+      <c r="G208" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="1" t="n">
+        <v>209</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="F209" s="3" t="n">
+        <v>43934</v>
+      </c>
+      <c r="G209" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5238,7 +5289,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:J157">
+  <autoFilter ref="A1:J192">
     <filterColumn colId="6">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>

<commit_message>
Issue-210 Allow for shift click to draw straight line from previous point in EPMD
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$192</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$157</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$192</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$J$130</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$153</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$124</definedName>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="334">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -1049,6 +1049,9 @@
   </si>
   <si>
     <t xml:space="preserve">List of images for image buttons.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allow for shift click to draw straigh line from previous point in EPMD</t>
   </si>
 </sst>
 </file>
@@ -1498,7 +1501,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A207" activeCellId="0" sqref="A207:B207"/>
+      <selection pane="bottomLeft" activeCell="A210" activeCellId="0" sqref="A210:B210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5279,6 +5282,20 @@
         <v>17</v>
       </c>
     </row>
+    <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="F210" s="3" t="n">
+        <v>43961</v>
+      </c>
+      <c r="G210" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5289,7 +5306,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:J192">
+  <autoFilter ref="A1:J157">
     <filterColumn colId="6">
       <customFilters and="true">
         <customFilter operator="equal" val="OPEN"/>

</xml_diff>